<commit_message>
last changes to TypesAbilities -> add choose ability
</commit_message>
<xml_diff>
--- a/CharacterGeneration 2.5/TypesAbilities.xlsx
+++ b/CharacterGeneration 2.5/TypesAbilities.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ZiCold\OneDrive\Numenera\CharacterGeneration 2.5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/272cbd6127da4c97/TRPGs - Numenera/NumeneraAppFiles/CharacterGeneration 2.5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="6_{314EC72C-2C92-4771-B4AA-B19D652E9D7C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C23B7D68-D986-41AE-B8B3-AB67F6C739FD}"/>
+  <xr:revisionPtr revIDLastSave="44" documentId="6_{314EC72C-2C92-4771-B4AA-B19D652E9D7C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{238DF31B-41D6-426C-9C9D-44D749F52795}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="468" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="468" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nano" sheetId="1" r:id="rId1"/>
@@ -20,18 +20,7 @@
     <sheet name="Delve" sheetId="5" r:id="rId5"/>
     <sheet name="Wright" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191028" iterateDelta="1E-4" calcCompleted="0"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="191028" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -80,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="383">
   <si>
     <t>Type</t>
   </si>
@@ -104,40 +93,6 @@
   </si>
   <si>
     <t>auto</t>
-  </si>
-  <si>
-    <t>Pools Starting Values: Might - 7, Speed - 9, Intellect - 12_x000D_
-_x000D_
-Bonus Pools Values: You get 6 additional points to divide among your stat Pools however you wish._x000D_
-_x000D_
-Effort: Your Effort is 1._x000D_
-_x000D_
-Genius: You have an Intellect Edge of 1, a Might Edge of 0, and a Speed Edge of 0._x000D_
-_x000D_
-Expert Cypher Use: You can bear three cyphers at a time._x000D_
-_x000D_
-Weapons: You can use light weapons without penalty. You have an inability with medium weapons and heavy weapons; your attacks with medium and heavy weapons are hindered._x000D_
-_x000D_
-Skills: You are trained in understanding numenera, inability in salvaging numenera, inability crafting numenera._x000D_
-_x000D_
-Starting Equipment: You start with clothing, one weapon, a book about the numenera, three cyphers (chosen for you by the GM), one oddity (chosen for you by the GM), and 4 shins (coins). Before selecting your weapons, armor, and other gear, you might want to wait until after you’ve chosen your esoteries, descriptor, and focus._x000D_
-_x000D_
-Community Scholar: While you are present within a community, and actively and personally working on behalf of that community, the community’s health and infrastructure are both increased by +1. Enabler._x000D_
-_x000D_
-Nano Player Intrusions: you can spend 1 XP to use one of the following player intrusions, provided the situation is appropriate and the GM agrees._x000D_
-- Advantageous Malfunction: a numenera device that is being used against you malfunctions. It might harm the user or one of their allies for a round, or activate a dramatic and distracting side effect for a few rounds._x000D_
-- Convenient Glimmer: a glimmer provides you with a clear answer or suggests a course of action with regard to an urgent question, problem, or obstacle you’re facing._x000D_
-- Inexplicably Unbroken: an inactive, ruined, or presumed-destroyed device temporarily activates and performs a useful function relevant to the situation. This is enough to buy you some time for a better solution, alleviate a complication that was interfering with your abilities, or just get you one more use out of a depleted cypher or artifact.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adept Cypher Use: You can bear four cyphers at a time.
-Improved Community Scholar: A community continues to modify its health and infrastructure by +1 rank. However, you do not need to be constantly present in and actively working on behalf of the community for it to gain this benefit; it gains it merely because of your past efforts on the community’s behalf. Enabler. </t>
-  </si>
-  <si>
-    <t>Master Cypher Use: You can bear five cyphers at a time.</t>
-  </si>
-  <si>
-    <t>Recruit Deputy: You gain a level 4 follower. They are not restricted on their modifications. Enabler.</t>
   </si>
   <si>
     <t>option</t>
@@ -352,53 +307,9 @@
     <t>Sculpt Flesh (2 Intellect points): You cause a willing creature’s fingers to lengthen into claws and her teeth to grow into fangs by sculpting her flesh. The effect lasts for ten minutes. The damage dealt by the target’s unarmed strikes increases to 4 points. Action.</t>
   </si>
   <si>
-    <t>Pools Starting Values: Might - 11, Speed - 10, Intellect - 7_x000D_
-_x000D_
-Bonus Pools Values: You get 6 additional points to divide among your stat Pools however you wish._x000D_
-_x000D_
-Effort: Your Effort is 1._x000D_
-_x000D_
-Fighter: You have a Might Edge of 1, a Speed Edge of 1, and an Intellect Edge of 0._x000D_
-_x000D_
-Combat Prowess: You add +1 damage to one type of attack of your choice: melee attacks or ranged attacks. Enabler._x000D_
-_x000D_
-Cypher Use: You can bear two cyphers at a time._x000D_
-_x000D_
-Trained in Armor: You can wear armor for long periods of time without tiring and can compensate for slowed reactions from wearing armor. You reduce the Speed Effort cost for wearing armor by 1. Enabler._x000D_
-_x000D_
-Weapons: You can use any weapon without penalty._x000D_
-_x000D_
-Physical Skills: Choose one of the following skills in which you aren’t already trained: balancing, climbing, jumping, or swimming. You are trained in this skill. You have an inability in crafting numenera, salvaging numenera, and understanding numenera._x000D_
-_x000D_
-Starting Equipment: You start with clothing, two weapons (or one weapon and a shield), light or medium armor, an explorer’s pack, two cyphers (chosen for you by the GM), one oddity (chosen for you by the GM), and 5 shins (coins). If you start with a ranged weapon that requires ammunition (arrows, for example), you start with 12 of that type of ammunition. Before selecting your weapons, armor, and other gear, you might want to wait until after you’ve chosen your fighting moves, descriptor, and focus._x000D_
-_x000D_
-Community Defender: While you are present within a community, and actively and personally working on behalf of that community, the community’s effective rank for damage inflicted is +1. Enabler. _x000D_
-_x000D_
-Player Intrusions: you can spend 1XP to use one of the following player intrusions, provided the situation is appropriate and the GM agrees. _x000D_
-- Perfect Setup: you’re fighting at least three foes and each one is standing in exactly the right spot for you to use a move you trained in long ago, allowing you to attack all three as a single action. Make a separate attack roll for each foe. You remain limited by the amount of Effort you can apply on one action. _x000D_
-- Old Friend: a comrade in arms from your past shows up unexpectedly and provides aid in whatever you’re doing. They are on a mission of their own and can’t stay longer than it takes to help out, chat a while after, and perhaps share a quick meal. _x000D_
-- Weapon Break: your foe’s weapon has a weak spot and in the course of the combat quickly becomes damaged and moves two steps down the object damage track.</t>
-  </si>
-  <si>
     <t>Skill With Attacks: Choose one type of attack in which you are not already trained: light bashing, light bladed, light ranged, medium bashing, medium bladed, medium ranged, heavy bashing, heavy bladed, or heavy ranged. You are trained in attacks using that type of weapon. Enabler.</t>
   </si>
   <si>
-    <t xml:space="preserve">Expert Cypher Use: You can bear three cyphers at a time.
-Skill With Attacks: Choose one type of attack in which you are not already trained: light bashing, light bladed, light ranged, medium bashing, medium bladed, medium ranged, heavy bashing, heavy bladed, or heavy ranged. You are trained in attacks using that type of weapon. Enabler.
-Improved Community Defender: A community continues to modify its effective rank for damage inflicted by +1. However, you do not need to be constantly present in and actively working on behalf of the community for it to gain this benefit; it gains it merely because of your past defense of the community. Enabler. 
-</t>
-  </si>
-  <si>
-    <t>Adept Cypher Use: You can bear four cyphers at a time.
-Mastery With Attacks: Choose one type of attack in which you are trained: light bashing, light bladed, light ranged, medium bashing, medium bladed, medium ranged, heavy bashing, heavy bladed, or heavy ranged. You are specialized in attacks using that type of weapon. Enabler. (In place of this ability, you may instead select Skill With Attacks to become trained in one type of attack.)</t>
-  </si>
-  <si>
-    <t>Mastery With Attacks: Choose one type of attack in which you are trained: light bashing, light bladed, light ranged, medium bashing, medium bladed, medium ranged, heavy bashing, heavy bladed, or heavy ranged. You are specialized in attacks using that type of weapon. Enabler. (In place of this ability, you may instead select Skill With Attacks to become trained in one type of attack.)
-Choose one of the following:
-- Rampaging Beast Horde (12 Might points): You can take community actions with a horde or a community as if you were a rank 3 rampaging beast horde for one hour. You can spend a few rounds or minutes here and there taking character actions if something requires attention and still retain your horde status. For each allied PC that joins you and remains with you during this period who also spends 12 points from one of their Pools, you can extend the duration by one hour. Each point of damage you take while being treated as a rampaging beast horde is deducted from your Might Pool, or if you have allied PCs helping, the damage is split up and deducted from all your Might Pools evenly. Action to initiate. 
-- Recruit Deputy: You gain a level 4 follower. They are not restricted on their modifications. Enabler.</t>
-  </si>
-  <si>
     <t>Fleet of Foot (1+ Speed points): You can move a short distance as part of another action. You can move a long distance as your entire action for a turn. If you apply a level of Effort to this ability, you can move a long distance and make an attack as your entire action for a turn, but the attack is hindered. Enabler.</t>
   </si>
   <si>
@@ -600,49 +511,6 @@
     <t>Surging Confidence (1 Might point): When you use an action to make your first recovery roll of the day, you immediately gain another action. Enabler.</t>
   </si>
   <si>
-    <t>Pools Starting Values: Might - 10, Speed - 10, Intellect - 10_x000D_
-_x000D_
-Bonus Pools Values: You get 6 additional points to divide among your stat Pools however you wish._x000D_
-_x000D_
-Effort: Your Effort is 1._x000D_
-_x000D_
-Jack of All Trades: You have an Edge of 1 for one stat of your choice: Might, Speed, or Intellect. You have an Edge of 0 for the other two stats._x000D_
-_x000D_
-Cypher Use: You can bear two cyphers at a time._x000D_
-_x000D_
-Weapons: You can use light and medium weapons without penalty. You have an inability with heavy weapons; your attacks with heavy weapons are hindered._x000D_
-_x000D_
-Skills: Choose one skill (other than attacks or defense) in which you aren’t already trained. You are trained in this skill._x000D_
-_x000D_
-Flex Skill: At the beginning of each day, choose one task (other than attacks or defense) on which you will concentrate. For the rest of that day, you’re trained in that task. You can’t use this ability with a skill you’re already trained in to become specialized._x000D_
-_x000D_
-Starting Equipment: You start with clothing, two weapons, light armor, an explorer’s pack, a pack of light tools, two cyphers (chosen for you by the GM), one oddity (chosen by the GM), and 8 shins. Before selecting your weapons, armor, and other gear, you might want to wait until after you’ve chosen your tricks of the trade, descriptor, and focus._x000D_
-_x000D_
-Community Fixer: While you are present within a community, and actively and personally working on behalf of that community, the community’s effective rank for health or infrastructure is increased by +1. You choose which is modified during any given community action. Enabler.Community Fixer: While you are present within a community, and actively and personally working on behalf of that community, the community’s effective rank for health or infrastructure is increased by +1. You choose which is modified during any given community action. Enabler.Community Fixer: While you are present within a community, and actively and personally working on behalf of that community, the community’s effective rank for health or infrastructure is increased by +1. You choose which is modified during any given community action. Enabler._x000D_
-_x000D_
-Jack Player Intrusions: you can spend 1 XP to use one of the following player intrusions, provided the situation is appropriate and the GM agrees._x000D_
-- Familiar Insight: you know this person (or heard about them somewhere) well enough to give insight about their motives or intentions and how best to convince them to see things your way. You know the right words, posturing, inflection, amount of emotional manipulation, or even what sort of joke or agreeable complaint might sway them. This can convince a neutral person to take your side, or a hostile one to hear you out for a little while longer._x000D_
-- Inspirational Recall: you recall an important detail from a previous encounter (perhaps something you don’t even remember noticing at the time) that suggests a successful course of action for your current situation. This might be recognizing a password hidden in an innocuous code or riddle, realizing you saw a suspicious individual near a crime scene, overhearing an important conversation between two NPCs, or understanding that an NPC’s subtle glance or gesture had additional connotations indicating what you should do._x000D_
-- Lucky Break: something unexpected happens that is to your advantage. A rope your opponent is hanging from might snap, the person you’re debating in front of an influential Aeon Priest might trip or forget what they were going to say, or something that was supposed to last only a round or two lasts a little while longer.</t>
-  </si>
-  <si>
-    <t>Skills: You are trained in one task of your choosing (other than attacks or defense). If you choose a task you’re already trained in, you become specialized in that task. You can’t choose a task you’re already specialized in.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Expert Cypher Use: You can bear three cyphers at a time.
-Skills: You are trained in one task of your choosing (other than attacks or defense). If you choose a task you’re already trained in, you become specialized in that task. You can’t choose a task you’re already specialized in.
-Improved Community Fixer: A community continues to modify its health or infrastructure by +1 rank. However, you do not need to be constantly present in and actively working on behalf of the community for it to gain this benefit; it gains it merely because of your past efforts on the community’s behalf. Whichever stat you modified last remains active until you return and modify it to something else. Enabler.
-</t>
-  </si>
-  <si>
-    <t>Adept Cypher Use: You can bear four cyphers at a time.
-Skills: You are trained in one task of your choosing (other than attacks or defense). If you choose a task you’re already trained in, you become specialized in that task. You can’t choose a task you’re already specialized in.</t>
-  </si>
-  <si>
-    <t>Skills: You are trained in one task of your choosing (other than attacks or defense). If you choose a task you’re already trained in, you become specialized in that task. You can’t choose a task you’re already specialized in.
-Recruit Deputy: You gain a level 4 follower. They are not restricted on their modifications. Enabler.</t>
-  </si>
-  <si>
     <t>Trained in Armor: You can wear armor for long periods of time without tiring and can compensate for slowed reactions from wearing armor. You can wear any kind of armor. You reduce the Speed Effort cost for wearing armor by 1. Enabler.</t>
   </si>
   <si>
@@ -832,40 +700,6 @@
     <t>Investigative Skills: You are trained in two skills in which you are not already trained. Choose two of the following: identifying, perception, lockpicking, or assessing danger. You can select this ability multiple times. Each time you select it, you must choose two different skills. Enabler.</t>
   </si>
   <si>
-    <t>Pools Starting Values: Might - 8, Speed - 9, Intellect - 11_x000D_
-_x000D_
-Bonus Pools Values: You get 6 additional points to divide among your stat Pools however you wish._x000D_
-_x000D_
-Effort: Your Effort is 1._x000D_
-_x000D_
-Leader: You have an Intellect Edge of 1, a Might Edge of 0, and a Speed Edge of 0._x000D_
-_x000D_
-Cypher Use: You can bear two cyphers at a time._x000D_
-_x000D_
-Weapons: You can use light weapons without penalty. You have an inability with medium and heavy weapons; your attacks with medium and heavy weapons are hindered._x000D_
-_x000D_
-Interaction Skills: You are trained in two skills in which you are not already trained. Choose two of the following: persuasion, negotiation, deceiving, public speaking, seeing through deception, or intimidating. You have an inability in crafting numenera, salvaging numenera, and understanding numenera. Enabler._x000D_
-_x000D_
-Community Leader: While you are present within a community, and actively and personally working on behalf of that community, the community’s rank is +1 for all purposes except damage inflicted. Enabler._x000D_
-Starting Equipment: You start with stylish clothing and a light weapon of your choice, two cyphers (chosen by the GM), one oddity, and 9 shins. If you start with a ranged weapon that requires ammunition (arrows, for example), you start with 12 of that type of ammunition. Before choosing your weapon and other gear, you might want to wait until after you’ve chosen your precepts, descriptor, and focus._x000D_
-_x000D_
-Arkus Player Intrusions: you can spend 1 XP to use one of the following player intrusions,_x000D_
-provided the situation is appropriate and the GM agrees._x000D_
-- Friendly NPC: an NPC you don’t know, someone you don’t know that well, or someone you know but who hasn’t been particularly friendly in the past chooses to help you, though doesn’t necessarily explain why. Maybe they’ll ask you for a favor in return afterward, depending on how much trouble they go to._x000D_
-- Perfect Suggestion: a follower or other already-friendly NPC suggests a course of action with regard to an urgent question, problem, or obstacle you’re facing._x000D_
-- Unexpected Gift: an NPC hands you a physical gift you were not expecting, one that helps put the situation at ease if things seem strained, or provides you with a new insight for understanding the context of the situation if there’s something you’re failing to understand or grasp.</t>
-  </si>
-  <si>
-    <t>Expert Cypher Use: You can bear three cyphers at a time.
-Improved Community Leader: A community continues to modify its effective rank by +1 for any task except for attack and defense. However, you do not need to be constantly present in and actively working on behalf of the community for it to gain this benefit; it gains it merely because of your past work in the community. Enabler.</t>
-  </si>
-  <si>
-    <t>Adept Cypher Use: You can bear four cyphers at a time.</t>
-  </si>
-  <si>
-    <t>Recruit Deputy: You gain a level 4 follower. They are not restricted on their modifications. Enabler. Alternatively, you can choose to advance a level 3 follower you already have to level 4 and then gain a new level 3 follower. Enabler.</t>
-  </si>
-  <si>
     <t>Anecdote (2 Intellect points): You can lift the spirits of a group of creatures and help them bond together by entertaining them with an uplifting or pointed anecdote. For the next hour, those who pay attention to your story are trained in a task you choose that’s related to the anecdote, as long as it’s not an attack or defense task. Action to initiate, one minute to complete.</t>
   </si>
   <si>
@@ -1020,40 +854,6 @@
   </si>
   <si>
     <t>Friendship (1 Intellect point): You convince a sentient creature to regard you positively, as they would a potential friend. You gain an asset in all future interactions with the creature until you give them a reason to no longer regard you well, at which point this effect ends. The affected creature isn't "charmed” supernaturally—they are not compelled or controlled in any way. So this isn't enough to keep a hostile foe from attacking, but it can help in a subsequent interaction task to do that.</t>
-  </si>
-  <si>
-    <t>Pools Starting Values: Might - 9, Speed - 9, Intellect - 10_x000D_
-_x000D_
-Bonus Pools Values: You get 6 additional points to divide among your stat Pools however you wish._x000D_
-_x000D_
-Effort: Your Effort is 1._x000D_
-_x000D_
-Talented: You have an Intellect Edge of 1, a Speed Edge of 1, and a Might Edge of 0._x000D_
-_x000D_
-Cypher Use: You can bear two cyphers at a time._x000D_
-_x000D_
-Weapons: You can use light and medium weapons without penalty. You have an inability with heavy weapons; your attacks with heavy weapons are hindered._x000D_
-_x000D_
-Skills: You are trained in salvaging numenera. In addition, you are trained in an exploration skill in which you are not already trained. Choose from the following: navigation, perception, sensing danger, creature knowledge, initiative, peacefully opening communications with strangers, or tracking. You have an inability in crafting numenera and understanding numenera. Enabler._x000D_
-_x000D_
-Community Explorer: While you are present within a community, and actively and personally working on behalf of that community, the community’s effective rank for purposes of finding resources, locating new trade routes, knowing about conditions just beyond the community, and detecting sneak attacks by enemies is +1. Enabler._x000D_
-Starting Equipment: You start with clothing,  two weapons (or one weapon and a shield), light armor or 1 extra unit of responsive synth (your choice), a pack of light tools, an explorer’s pack, two cyphers (chosen by the GM), one oddity (chosen by the GM), and 3 shins (coins). If you start with a ranged weapon that requires ammunition (arrows, for example), you start with 12 of that type of ammunition. Before selecting your weapons, armor, and other gear, you might want to wait until after you’ve chosen your Delve lore, descriptor, and focus._x000D_
-_x000D_
-Delve Player Intrusions: you can spend 1 XP to use one of the following player intrusions, provided the situation is appropriate and the GM agrees._x000D_
-- Fortuitous Malfunction: a trap or a dangerous device malfunctions before it can affect you._x000D_
-- Serendipitous Landmark: just when it seems like the path is lost, or you are, a trail marker, landmark, or simply the way the terrain or corridor bends, rises, or falls away suggests to you the best path forward, at least from this point._x000D_
-- Weak Strain: the poison or disease turns out not to be as debilitating or deadly as it first seemed, and inflicts only half the damage that it would have otherwise.</t>
-  </si>
-  <si>
-    <t>Expert Cypher Use: You can bear three cyphers at a time.
-Improved Community Explorer: A community continues to modify its rank by +1 on any task that involves finding resources, locating new trade routes, knowing about conditions just beyond the community, and detecting sneak attacks by enemies. However, you do not need to be constantly present in and actively working on behalf of the community for it to gain this benefit; it gains it merely because of your past efforts in the community. Enabler.</t>
-  </si>
-  <si>
-    <t>Iotum Cache: Whenever you find or salvage iotum, you gain an additional result on the Iotum Result Table. Enabler.</t>
-  </si>
-  <si>
-    <t>Adept Cypher Use: You can bear four cyphers at a time.
-Refine Iotum: When you discover iotum on an initial salvage task, your follow-up attempts to locate a specific variety of iotum gain one free level of Effort if you use at least one level of Effort (maximum six levels). Enabler.</t>
   </si>
   <si>
     <t>Additional Training: You are trained in two additional skills in which you are not already trained. Choose from the following: navigation, perception, sensing danger, initiative, peacefully opening communications with strangers, and tracking. Enabler.</t>
@@ -1144,9 +944,6 @@
     <t>Scan for Iotum (2 Intellect points): Using a device or some kind of unique sense, you scan an area equal in size to a 10-foot (3 m) cube, including all objects or structures. The area must be within immediate range. The difficulty of the task is equal to the level of the object or structure being scanned. Scanning in this fashion eases initial salvage task in the area to determine if anything is worth salvaging. This ability doesn’t improve your ability to find a specific kind of iotum, only to discover whether there is iotum within the salvage source in the first place. That said, many materials and energy fields prevent or resist scanning. Action.</t>
   </si>
   <si>
-    <t>Deconstruct (3 Intellect points): You take the time to closely study a bit of scrap, machine, cypher, artifact, or other numenera object or structure before attempting to salvage iotum from it. If the salvage source possesses iotum that can be salvaged (as determined by the GM) you gain one additional kind of iotum from the salvage attempt. Action to initiate, ten minutes to complete.</t>
-  </si>
-  <si>
     <t>Controlled Fall: When you fall while you are able to use actions and within reach of a vertical surface, you can attempt to slow your fall. Make a Speed roll. The difficulty is 1 for every 20 feet (6 m) you fall. On a success, you take half damage from the fall. If you reduce the difficulty to 0, you take no damage. Enabler.</t>
   </si>
   <si>
@@ -1204,177 +1001,376 @@
     <t>Trapster: You are trained in creating simple traps for human-sized or smaller targets. When you lay a trap, decide whether you want to hold the victim in place (a snare) or inflict damage (a deadfall). Creating a snare is a difficulty 3 task, while the difficulty of creating a deadfall is equal to the number of points of damage you want it to inflict. On a success, you create one-use trap in about one minute, and it is considered level 3 for the purposes of avoiding detection before it is sprung and for a victim trying to struggle free (if a snare). For each additional hour and level of Effort you can increase trap level up to 5. Action to initiate, one minute or one hour to complete.</t>
   </si>
   <si>
-    <t>Pools Starting Values: Might - 9, Speed - 7, Intellect - 12_x000D_
-_x000D_
-Bonus Pools Values: You get 6 additional points to divide among your stat Pools however you wish._x000D_
-_x000D_
-Effort: Your Effort is 1._x000D_
-_x000D_
-Inventor: You have an Intellect Edge of 1, a Might Edge of 0, and a Speed Edge of 0._x000D_
-_x000D_
-Cypher Use: You can bear three cyphers at a time._x000D_
-_x000D_
-Weapons: You can use light weapons without penalty. You have an inability with medium and heavy weapons; your attacks with medium and heavy weapons are hindered._x000D_
-_x000D_
-Skills: You are trained in crafting numenera. In addition, you are trained in a crafting skill in which you are not already trained. Choose one of the following: salvaging numenera, understanding numenera, engineering, woodcrafting, armoring, weaponsmithing, or another crafting skill of your choice. You have an inability in salvaging numenera and understanding numenera. Enabler._x000D_
-_x000D_
-Community Builder: While you are present within the community, and actively and personally working on behalf of that community, +3 is added to the community’s infrastructure. Enabler._x000D_
-_x000D_
-Always Tinkering: If you have any tools and materials at all, and you are carrying fewer cyphers than your limit, you can create a cypher if you have an hour of time to spend. The new cypher is random and always 2 levels lower than normal (minimum 1). It’s also temperamental and fragile. These are called temperamental cyphers. If you give it to anyone else to use, it falls apart immediately, useless. The base materials required for Always Tinkering could include a wide variety of things, including scrap, burned-out (used) cyphers, or actual iotum and parts. In the latter case, only 1 unit of iotum and 1 point worth of parts is used to create the temperamental cypher. Action to initiate, one hour to complete._x000D_
-_x000D_
-Numenera Plans: You start with two numenera plans of your choice. Enabler._x000D_
-_x000D_
-Starting Equipment: You start with clothing, one weapon, an explorer’s pack, a book about crafting, three cyphers (chosen by the GM), one oddity (chosen by the GM), a box of crafting tools, and 5 shins (coins). If you start with a ranged weapon that requires ammunition (arrows, for example), you start with 12 of that type of ammunition. Before selecting your weapons, armor, and other gear, you might want to wait until after you’ve chosen your abilities, descriptor, and focus._x000D_
-_x000D_
-Starting Iotum: In addition to your starting equipment, you start with 4 units of io and 4 units of responsive synth. You also have 6 units of parts._x000D_
-_x000D_
-Wright Player Intrusions: you can spend 1 XP to use one of the following player intrusions, provided the situation is appropriate and the GM agrees._x000D_
-- Device Perfection: a device or installation works even better than you expected it would, at least in this instance. Maybe the range is twice as long, the duration is 100% longer, or the effect itself is 50% stronger._x000D_
-- Crafting Insight: you are inspired, and you finish crafting the object or structure earlier than was expected (maybe even halving the total time)._x000D_
-- Tinkering Vision: when using your Always Tinkering special ability, you discover that the materials you’re using are of unexpectedly high quality, giving you specific options to choose from. So instead of gaining a random cypher, you gain the cypher of your choice (though it’s still a temperamental cypher, so it’s 2 levels lower than normal and you can’t give it to someone else without destroying it).</t>
-  </si>
-  <si>
-    <t>Numenera Plans: You gain two additional numenera plans of your choice. Enabler.</t>
+    <t>Additional Numenera Plans: You gain two additional numenera plans. You can take this ability multiple times. When you advance to a higher tier and have the option of replacing one of your existing inspired techniques, you can't replace Additional Numenera Plans. Enabler.</t>
+  </si>
+  <si>
+    <t>Additional Training: You are trained in two additional crafting skills of your choice. Enabler.</t>
+  </si>
+  <si>
+    <t>Adept Builder: When you attempt a crafting task, you lower the assessed difficulty for creating a complex object or structure by one step. For example, if the assessed difficulty for creating a level 3 installation would normally be 6, for you the assessed difficulty is 5 (this also reduces the crafting time). If you’re trained or specialized in a relevant crafting skill (which you likely are), that could reduce the assessed crafting difficulty to 4 or 3, also reducing the time to build even more. Enabler.</t>
+  </si>
+  <si>
+    <t>Boost Artifact (2 Intellect points): An artifact you activate with your next action functions as if it were two levels higher. Action.</t>
+  </si>
+  <si>
+    <t>Inspired Techniques: Choose one of the following inspired techniques (or an inspired technique from a lower tier) to add to your repertoire. In addition, you can replace one of your lower-tier inspired techniques with a different inspired technique from the same lower tier.</t>
+  </si>
+  <si>
+    <t>Juggernaut (9 Intellect points): You call upon your connection to one installation you’ve built or repaired to become a singleuse weapon of immense destruction, though this also destroys the installation. While you are within a community that currently benefits from your Community Builder or Improved Community Builder ability, you can select an installation of level 5 or higher within very long range. The installation launches itself like a massive missile at a target you specify within very long range of the installation and then detonates, inflicting 20 points of damage on all targets within short range. This destroys the installation. Targets who successfully defend still suffer 8 points of damage. Action.</t>
+  </si>
+  <si>
+    <t>Extra Use (3 Intellect points): You attempt to gain an extra use from an installation or artifact without triggering a depletion roll. The difficulty of the task is equal to the level of the installation or artifact. If you crafted the installation or artifact, you gain an asset to the task. On a failure, the depletion roll occurs normally. You could also try to use a cypher without burning it out, but the task is hindered. A failed attempt to gain an additional use from a cypher destroys it before it can produce the desired effect. Action.</t>
+  </si>
+  <si>
+    <t>Boost Cypher (2 Intellect points): The cypher you activate with your next action functions as if it were 2 levels higher. Action.</t>
+  </si>
+  <si>
+    <t>Community Awareness (4 Intellect points): While you are within a community that currently benefits from your Community Builder or Improved Community Builder ability, you can ask the GM a very simple, general question about that general area, such as “Are there enemies trying to sneak over the wall?” or “Is someone watching the flower shop?” or “Is there a Nano sensor active by my home?” If the answer you seek is not in the area, you receive no information. Action.</t>
+  </si>
+  <si>
+    <t>Confounding Jargon (4 Intellect points): You begin to discuss the intricacies of crafting numenera, which goes completely over the heads of most creatures but is sufficient to distract a target within immediate range until your next turn. You and each of your allies gain an asset on one interaction, attack, or defense task associated with the target before your next turn. This ability doesn’t work on creatures you can’t talk with. Action.</t>
+  </si>
+  <si>
+    <t>Boost Cypher Function (4 Intellect points): Add 3 to the functioning level of a cypher that you activate with your next action, or change one aspect of its parameters (range, duration, area, etc.) by up to double or down to one tenth. Action.</t>
+  </si>
+  <si>
+    <t>Master Machine (8 Intellect points): You can control the functions of a machine you have bonded with, including installations, intelligent or otherwise. In addition, if you use an action to concentrate on a machine, you are aware of what is going on around it (you see and hear as if you were standing next to it, no matter how far away you are). You must touch the machine to create the bond, but afterward, there is no range limitation. This bond lasts for one week. You can bond with only one machine at a time. Action to initiate.</t>
+  </si>
+  <si>
+    <t>Natural Crafter: All commonplace objects or structures you craft are effectively 1 level higher than an average example of that object or structure. For instance, if you craft a defensive wall that would normally be level 4, its effective level is 5. Enabler.</t>
+  </si>
+  <si>
+    <t>Disable Machine (3+ Intellect points): With a few deft touches, you infuse a powered device of level 3 or lower with conflicting instructions. If affected, the device is destroyed or disabled for at least one minute, depending on its size and complexity. The GM may rule that the disabling effect lasts until the device is repaired. In addition to the normal options for using Effort, you can also choose to use Effort to increase the maximum level of the target by 1 for each level applied. Thus, to overload a level 5 device (two levels above the normal limit), you must apply two levels of Effort. Action.</t>
+  </si>
+  <si>
+    <t>Device Insight (3+ Intellect points): When examining any numenera device, you can ask the GM one question about the device to gain an idea of its capabilities or functions, how it can be activated or deactivated, what its weakness is, how it can be repaired, or any other similar query. This ability is for difficult or strange things beyond those readily identified by understanding numenera. The GM may require a roll whose difficulty is equal to the device’s level; however, you gain two assets to any such task, and training in the understanding numenera skill also applies. Each time you use this ability on the same device after the first use, you must apply one additional level of Effort. Action.</t>
+  </si>
+  <si>
+    <t>Energy Redirection (5+ Intellect points): You take the time to closely study a bit of scrap, machine, cypher, artifact, or other numenera object or structure. When you’ve finished, you can drain the energy from it and redirect it elsewhere. Iotum are burned out. Cyphers are rendered useless. Artifacts, installations, vehicles, and automatons must make a depletion roll. You can redirect the energy from the target object to restore 1 Might point per level of the target object. Alternatively, you can redirect the energy into a depleted cypher, artifact, installation, vehicle, or automaton that has a level equal to or less than the drained object. If the device isn’t broken, it gains one additional use and then becomes depleted and broken. Each additional level of Effort you apply increases the maximum level of the object you can recharge. Action to initiate, ten minutes to complete.</t>
+  </si>
+  <si>
+    <t>Faster Builder: When you attempt a crafting task, you lower the assessed difficulty for creating a complex object or structure by two steps. (This replaces Adept Builder, if you took that; you can exchange that ability for another tier 3 inspired technique.) Enabler.</t>
+  </si>
+  <si>
+    <t>Rapid Builder: When you attempt a crafting task, you lower the assessed difficulty for creating a complex object or structure by three steps. (This replaces Adept Builder and Faster Builder, if you took either of those; you can exchange those abilities for another tier 3 and tier 5 inspired technique.) Enabler.</t>
+  </si>
+  <si>
+    <t>Right Tool for the Job (1 Intellect point + iotum): If you have at least 1 unit of iotum, you can fashion a temporary device that provides an asset to one physical, noncombat task, identified ahead of time. For example, if you need to climb a wall, you could create some sort of climbing assistance device; if you need to break out of a cell, you can tune iotum in your possession to serve as a lockpick; if you need to create a small distraction, you could trigger an iotum to make a loud bang and flash; and so on. Once fashioned, the adapted iotum lasts for about a minute or until used for the intended purpose. This use destroys the iotum. Action to prepare the iotum; action to initiate.</t>
+  </si>
+  <si>
+    <t>Impressive Device (3 Intellect points or iotum): If you have at least 1 unit of iotum, you can fashion a temporary device that causes some kind of impressive visual or audio display, such as colored lights that form a tracery over your entire body and change according to your mood and desire. The effect lasts for one minute. During this period, all your interaction tasks gain an asset. Once fashioned, the adapted iotum lasts for about a minute or until used for the intended purpose. This does not destroy the iotum. Alternatively, you can choose to have this destroy the iotum, in which case there is no Intellect cost. Action to prepare the iotum; action to initiate.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Follower: You gain a level 2 follower. One of their modifications must be for crafting, such as crafting numenera. You can take this ability multiple times, each time gaining another level 2 follower. The GM may require that you spend time seeking out a suitable follower as a long-term task as opposed to merely gaining one. Enabler. </t>
+  </si>
+  <si>
+    <t>Expert Crafter: Instead of rolling, you can choose to automatically succeed on a crafting task or subtask you’re trained in. The task must be difficulty 4 or lower. Enabler.</t>
+  </si>
+  <si>
+    <t>Improved Follower: You gain a level 3 follower. They are not restricted on their modifications. You can take this ability multiple times, each time gaining another level 3 follower. Alternatively, you could choose to advance a level 2 follower you already have to level 3 and then gain a new level 2 follower. Enabler.</t>
+  </si>
+  <si>
+    <t>Summon Sferic (8+ Intellect points): A sferic (Destiny, page 275) appears within a few days after you construct a simple beacon designed as a lure. If you apply an additional level of Effort as part of the call, the sferic is amenable to your instructions toward building an object or structure; otherwise, it acts according to its nature (which means it might still build something for you, but you risk havingyour mind plucked from your head when you make your request). The sferic remains until it finishes creating the structure you asked of it or it is attacked (in which case it defends itself and then leaves). Action to initiate, three days to construct beacon and summon sferic.</t>
+  </si>
+  <si>
+    <t>Scramble Machine (2 Intellect points): You render one machine within short range unable to function for one round. Alternatively, you can hinder any action by the machine (or by someone attempting to use the machine) for one minute. Action.</t>
+  </si>
+  <si>
+    <t>Interaction Skills: You are trained in two skills in which you are not already trained. Choose two of the following: deceiving, persuading, public speaking, seeing through deception, or intimidating. You can select this ability multiple times. Each time you select it, you must choose two different skills. Enabler.</t>
+  </si>
+  <si>
+    <t>Modify Cyphers: You can take any two cyphers and quickly jury-rig a new cypher of the same level as the lowest-level cypher. You determine the function of the new cypher, but it must be that of a cypher you have used before (but not necessarily one for which you have plans). The new cypher is a temperamental cypher, like those created with your Always Tinkering ability. The original two cyphers are consumed in this process. This ability does not function if one or more of the original cyphers are temperamental. Action.</t>
+  </si>
+  <si>
+    <t>Knowing the Weak Points: You gain +3 damage when attempting to damage a device, automaton, or other machine. Enabler.</t>
+  </si>
+  <si>
+    <t>Modify Artifact Function (5 Intellect points): You can take an artifact and any two cyphers and quickly jury-rig a new artifact of the level of the lowest-level cypher. You determine the function of the new artifact, but it must be that of an artifact or cypher you have used before (but not necessarily one for which you have plans). The GM sets the depletion of the new artifact, if applicable (it will usually be a bit worse than the original artifact). The two cyphers and the original artifact are consumed in this process. The original cyphers cannot be temperamental cyphers. Action.</t>
+  </si>
+  <si>
+    <t>Usurp Cypher: Choose one cypher that you carry. The cypher must have an effect that is not instantaneous. You destroy the cypher and gain its power, which functions for you continuously. You can choose a cypher when you gain this ability, or you can wait and make the choice later. However, once you usurp a cypher’s power, you cannot later switch to a different cypher—the ability works only once. Action to initiate.</t>
+  </si>
+  <si>
+    <t>Trigger Iotum Ray (1 Intellect point or iotum): If you have at least 1 unit of iotum, you can trigger it to release a short-range ray of force that inflicts 3 points of damage. This does not destroy the iotum. Alternatively, you can choose to have this destroy the iotum, in which case there is no Intellect cost. Action.</t>
+  </si>
+  <si>
+    <t>Knowledge Skills: You are trained in two skills in which you are not already trained. Choose two areas of knowledge such as history, geography, archeology, and so on. You can select this ability multiple times. Each time you select it, you must choose two different skills. Enabler.</t>
+  </si>
+  <si>
+    <t>Quick Armoring (4 Intellect points + io): You can siphon the residual energy in io (the eponymous iotum) to integrate and reinforce a layer of tightly wrapped clothing or encompassing cloaks that you wear. This requires at least one io, although it is not consumed in the process. For the next hour, you gain +2 to Armor. Action to initiate, one minute to complete.</t>
+  </si>
+  <si>
+    <t>Machine Bond: From very long range, you can activate and control a device (including an installation, automaton, or vehicle) that you have bonded with. For example, you can detonate a cypher even when it is held by someone else, or cause an installation turret to fire where you direct. Bonding is a process that requires 28 hours of meditation in the presence of the machine. Action.</t>
+  </si>
+  <si>
+    <t>Modify Artifact Power (6 Intellect points): You permanently add +1 to the level of an artifact of up to level 5. The difficulty of this task is equal to the modified higher level of the artifact. If the task is failed, the artifact makes a depletion roll and is not advanced in level. Once modified, the artifact can’t be similarly boosted again. Action.</t>
+  </si>
+  <si>
+    <t>Trained in Armor: You can wear armor for long periods of time without tiring and can compensate for slowed reactions from wearing armor. You can wear any kind of armor. You reduce the Speed Effort cost for wearing armor by 1. If you choose this as one of your starting inspired techniques, you start the game with armor of your choice. Enabler.</t>
+  </si>
+  <si>
+    <t>Make Do With Available Iotum (3+ Intellect points): Given an hour or so, you can figure out a way to substitute one kind of iotum called for in a plan with another kind of iotum, as long as the iotum you use is at least 1 level higher than the iotum originally called for. Alternatively, you can make do with 1 unit less than the number of units called for by the plan (to a minimum of 1 unit). For each additional level of Effort you apply, you can reduce the number by an additional unit, to a minimum of 1 unit. You can never substitute more than one kind of iotum per individual crafting task, though you could simultaneously substitute an iotum and decrease the number of units required by applying additional Effort. Action to initiate, one hour to complete.</t>
+  </si>
+  <si>
+    <t>Skill with Attacks: Choose one type of attack in which you are not already trained: light bashing, light bladed, light ranged, medium bashing, medium bladed, medium ranged, heavy bashing, heavy bladed, or heavy ranged. You are trained in attacks using that type of weapon. You can select this ability multiple times. Each time you select it, you must choose a different type of attack. Enabler.</t>
+  </si>
+  <si>
+    <t>Quick Mind Boost: You can siphon the residual energy in a single iotum to enhance your Intellect Edge by +1 for one minute. The iotum is destroyed. This ability does not allow you to enhance your Edge by more than +1. Action.</t>
+  </si>
+  <si>
+    <t>Town Pride: While you’re in a community that currently benefits from your Community Builder or Improved Community Builder special ability, your Might Edge, Speed Edge, and Intellect Edge all increase by 1. When you make a recovery roll in this community, you recover twice as many points. You can gain the benefit of this inspired technique even if you’re not in the community, as long as you have visited within the last three days. Enabler.</t>
+  </si>
+  <si>
+    <t>Pools Starting Values: Might - 9, Speed - 7, Intellect - 12
+Bonus Pools Values: You get 6 additional points to divide among your stat Pools however you wish.
+Effort: Your Effort is 1.
+Inventor: You have an Intellect Edge of 1, a Might Edge of 0, and a Speed Edge of 0.
+Cypher Use: You can bear three cyphers at a time.
+Weapons: You can use light weapons without penalty. You have an inability with medium and heavy weapons; your attacks with medium and heavy weapons are hindered.
+Skills: You are trained in crafting numenera. In addition, you are trained in a crafting skill in which you are not already trained. Choose one of the following: salvaging numenera, understanding numenera, engineering, woodcrafting, armoring, weaponsmithing, or another crafting skill of your choice. You have an inability in salvaging numenera and understanding numenera. Enabler.
+Community Builder: While you are present within the community, and actively and personally working on behalf of that community, +3 is added to the community’s infrastructure. Enabler.
+Artefact: You start with numenera plan of the artefact up to 1d6 level. This plan requires only half of resources to build the artefact. Chosen artefact plan is subject to GM approval.
+Starting Equipment: You start with clothing, one weapon, an explorer’s pack, a book about crafting, three cyphers (chosen by the GM), one oddity (chosen by the GM), a box of crafting tools, and 5 shins (coins). If you start with a ranged weapon that requires ammunition (arrows, for example), you start with 12 of that type of ammunition. Before selecting your weapons, armor, and other gear, you might want to wait until after you’ve chosen your abilities, descriptor, and focus.
+Starting Iotum: In addition to your starting equipment, you start with 4 units of io and 4 units of responsive synth. You also have 6 units of parts.
+Inspired Techniques: You have a special talent for crafting and can create objects and structures that others can barely imagine. These talents are called inspired techniques. Some inspired techniques are constant, ongoing effects, and others are specific actions that usually cost points from one of your stat Pools. You gain some of your inspired techniques using special numenera tools. For instance, when you use Scan for Iotum, it’s probably from a device that you’ve either made, found, or been given.
+Choose two of the inspired techniques described below. You can’t choose the same inspired technique more than once unless its description says otherwise. You can keep track of these in the Special Abilities section of your character sheet.
+Wright Player Intrusions: you can spend 1 XP to use one of the following player intrusions, provided the situation is appropriate and the GM agrees.
+- Device Perfection: a device or installation works even better than you expected it would, at least in this instance. Maybe the range is twice as long, the duration is 100% longer, or the effect itself is 50% stronger.
+- Crafting Insight: you are inspired, and you finish crafting the object or structure earlier than was expected (maybe even halving the total time).
+- Tinkering Vision: you know exactly what cypher can help with task at hand. You know that you have all right instruments and high quality parts. This cypher will be temperamental and will only work in your hands. To power it up you need at least 1 unit of iotum and/or burned-out (used) cypher. Time to make it depends on the situation, but no more than 1 hour.</t>
+  </si>
+  <si>
+    <t>Artefact: You start with numenera plan of the artefact up to 1d6 + 1 level. This plan requires only half of resources to build the artefact. Chosen artefact plan is subject to GM approval.
+Inspired Techniques: Choose one of the following inspired techniques (or an inspired technique from the first tier) to add to your repertoire. In addition, you can replace one of your first-tier inspired techniques with a different inspired technique from the first tier.</t>
   </si>
   <si>
     <t>Expert Cypher Use: You can bear four cyphers at a time.
 Improved Community Builder: A community continues to gain +3 to infrastructure due to your influence. However, you do not need to be constantly present in and actively working on behalf of the community for it to gain this benefit; it gains it merely because of your past crafting work in the community. Enabler.
-Numenera Plans: You gain two additional numenera plans of your choice. Enabler.</t>
+Artefact: You start with numenera plan of the artefact up to 1d6 + 2 level. This plan requires only half of resources to build the artefact. Chosen artefact plan is subject to GM approval.
+Inspired Techniques: Choose one of the following inspired techniques (or an inspired technique from a lower tier) to add to your repertoire. In addition, you can replace one of your lower-tier inspired techniques with a different inspired technique from the same lower tier.</t>
+  </si>
+  <si>
+    <t>Artefact: You start with numenera plan of the artefact up to 1d6 + 3 level. This plan requires only half of resources to build the artefact. Chosen artefact plan is subject to GM approval.
+Inspired Techniques: Choose one of the following inspired techniques (or an inspired technique from a lower tier) to add to your repertoire. In addition, you can replace one of your lower-tier inspired techniques with a different inspired technique from the same lower tier.</t>
   </si>
   <si>
     <t>Master Cypher Use: You can bear five cyphers at a time.
-Numenera Plans: You gain two additional numenera plans of your choice. Enabler.</t>
-  </si>
-  <si>
-    <t>Numenera Plans: You gain two additional numenera plans of your choice. Enabler.
-Recruit Deputy: You gain a level 4 follower. They are not restricted on their modifications. Enabler.</t>
-  </si>
-  <si>
-    <t>Additional Numenera Plans: You gain two additional numenera plans. You can take this ability multiple times. When you advance to a higher tier and have the option of replacing one of your existing inspired techniques, you can't replace Additional Numenera Plans. Enabler.</t>
-  </si>
-  <si>
-    <t>Additional Training: You are trained in two additional crafting skills of your choice. Enabler.</t>
-  </si>
-  <si>
-    <t>Adept Builder: When you attempt a crafting task, you lower the assessed difficulty for creating a complex object or structure by one step. For example, if the assessed difficulty for creating a level 3 installation would normally be 6, for you the assessed difficulty is 5 (this also reduces the crafting time). If you’re trained or specialized in a relevant crafting skill (which you likely are), that could reduce the assessed crafting difficulty to 4 or 3, also reducing the time to build even more. Enabler.</t>
-  </si>
-  <si>
-    <t>Boost Artifact (2 Intellect points): An artifact you activate with your next action functions as if it were two levels higher. Action.</t>
-  </si>
-  <si>
-    <t>Inspired Techniques: Choose one of the following inspired techniques (or an inspired technique from a lower tier) to add to your repertoire. In addition, you can replace one of your lower-tier inspired techniques with a different inspired technique from the same lower tier.</t>
-  </si>
-  <si>
-    <t>Juggernaut (9 Intellect points): You call upon your connection to one installation you’ve built or repaired to become a singleuse weapon of immense destruction, though this also destroys the installation. While you are within a community that currently benefits from your Community Builder or Improved Community Builder ability, you can select an installation of level 5 or higher within very long range. The installation launches itself like a massive missile at a target you specify within very long range of the installation and then detonates, inflicting 20 points of damage on all targets within short range. This destroys the installation. Targets who successfully defend still suffer 8 points of damage. Action.</t>
-  </si>
-  <si>
-    <t>Extra Use (3 Intellect points): You attempt to gain an extra use from an installation or artifact without triggering a depletion roll. The difficulty of the task is equal to the level of the installation or artifact. If you crafted the installation or artifact, you gain an asset to the task. On a failure, the depletion roll occurs normally. You could also try to use a cypher without burning it out, but the task is hindered. A failed attempt to gain an additional use from a cypher destroys it before it can produce the desired effect. Action.</t>
-  </si>
-  <si>
-    <t>Boost Cypher (2 Intellect points): The cypher you activate with your next action functions as if it were 2 levels higher. Action.</t>
-  </si>
-  <si>
-    <t>Community Awareness (4 Intellect points): While you are within a community that currently benefits from your Community Builder or Improved Community Builder ability, you can ask the GM a very simple, general question about that general area, such as “Are there enemies trying to sneak over the wall?” or “Is someone watching the flower shop?” or “Is there a Nano sensor active by my home?” If the answer you seek is not in the area, you receive no information. Action.</t>
-  </si>
-  <si>
-    <t>Confounding Jargon (4 Intellect points): You begin to discuss the intricacies of crafting numenera, which goes completely over the heads of most creatures but is sufficient to distract a target within immediate range until your next turn. You and each of your allies gain an asset on one interaction, attack, or defense task associated with the target before your next turn. This ability doesn’t work on creatures you can’t talk with. Action.</t>
-  </si>
-  <si>
-    <t>Boost Cypher Function (4 Intellect points): Add 3 to the functioning level of a cypher that you activate with your next action, or change one aspect of its parameters (range, duration, area, etc.) by up to double or down to one tenth. Action.</t>
-  </si>
-  <si>
-    <t>Master Machine (8 Intellect points): You can control the functions of a machine you have bonded with, including installations, intelligent or otherwise. In addition, if you use an action to concentrate on a machine, you are aware of what is going on around it (you see and hear as if you were standing next to it, no matter how far away you are). You must touch the machine to create the bond, but afterward, there is no range limitation. This bond lasts for one week. You can bond with only one machine at a time. Action to initiate.</t>
-  </si>
-  <si>
-    <t>Natural Crafter: All commonplace objects or structures you craft are effectively 1 level higher than an average example of that object or structure. For instance, if you craft a defensive wall that would normally be level 4, its effective level is 5. Enabler.</t>
-  </si>
-  <si>
-    <t>Disable Machine (3+ Intellect points): With a few deft touches, you infuse a powered device of level 3 or lower with conflicting instructions. If affected, the device is destroyed or disabled for at least one minute, depending on its size and complexity. The GM may rule that the disabling effect lasts until the device is repaired. In addition to the normal options for using Effort, you can also choose to use Effort to increase the maximum level of the target by 1 for each level applied. Thus, to overload a level 5 device (two levels above the normal limit), you must apply two levels of Effort. Action.</t>
-  </si>
-  <si>
-    <t>Device Insight (3+ Intellect points): When examining any numenera device, you can ask the GM one question about the device to gain an idea of its capabilities or functions, how it can be activated or deactivated, what its weakness is, how it can be repaired, or any other similar query. This ability is for difficult or strange things beyond those readily identified by understanding numenera. The GM may require a roll whose difficulty is equal to the device’s level; however, you gain two assets to any such task, and training in the understanding numenera skill also applies. Each time you use this ability on the same device after the first use, you must apply one additional level of Effort. Action.</t>
-  </si>
-  <si>
-    <t>Energy Redirection (5+ Intellect points): You take the time to closely study a bit of scrap, machine, cypher, artifact, or other numenera object or structure. When you’ve finished, you can drain the energy from it and redirect it elsewhere. Iotum are burned out. Cyphers are rendered useless. Artifacts, installations, vehicles, and automatons must make a depletion roll. You can redirect the energy from the target object to restore 1 Might point per level of the target object. Alternatively, you can redirect the energy into a depleted cypher, artifact, installation, vehicle, or automaton that has a level equal to or less than the drained object. If the device isn’t broken, it gains one additional use and then becomes depleted and broken. Each additional level of Effort you apply increases the maximum level of the object you can recharge. Action to initiate, ten minutes to complete.</t>
-  </si>
-  <si>
-    <t>Faster Builder: When you attempt a crafting task, you lower the assessed difficulty for creating a complex object or structure by two steps. (This replaces Adept Builder, if you took that; you can exchange that ability for another tier 3 inspired technique.) Enabler.</t>
-  </si>
-  <si>
-    <t>Rapid Builder: When you attempt a crafting task, you lower the assessed difficulty for creating a complex object or structure by three steps. (This replaces Adept Builder and Faster Builder, if you took either of those; you can exchange those abilities for another tier 3 and tier 5 inspired technique.) Enabler.</t>
-  </si>
-  <si>
-    <t>Right Tool for the Job (1 Intellect point + iotum): If you have at least 1 unit of iotum, you can fashion a temporary device that provides an asset to one physical, noncombat task, identified ahead of time. For example, if you need to climb a wall, you could create some sort of climbing assistance device; if you need to break out of a cell, you can tune iotum in your possession to serve as a lockpick; if you need to create a small distraction, you could trigger an iotum to make a loud bang and flash; and so on. Once fashioned, the adapted iotum lasts for about a minute or until used for the intended purpose. This use destroys the iotum. Action to prepare the iotum; action to initiate.</t>
-  </si>
-  <si>
-    <t>Impressive Device (3 Intellect points or iotum): If you have at least 1 unit of iotum, you can fashion a temporary device that causes some kind of impressive visual or audio display, such as colored lights that form a tracery over your entire body and change according to your mood and desire. The effect lasts for one minute. During this period, all your interaction tasks gain an asset. Once fashioned, the adapted iotum lasts for about a minute or until used for the intended purpose. This does not destroy the iotum. Alternatively, you can choose to have this destroy the iotum, in which case there is no Intellect cost. Action to prepare the iotum; action to initiate.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Follower: You gain a level 2 follower. One of their modifications must be for crafting, such as crafting numenera. You can take this ability multiple times, each time gaining another level 2 follower. The GM may require that you spend time seeking out a suitable follower as a long-term task as opposed to merely gaining one. Enabler. </t>
-  </si>
-  <si>
-    <t>Expert Crafter: Instead of rolling, you can choose to automatically succeed on a crafting task or subtask you’re trained in. The task must be difficulty 4 or lower. Enabler.</t>
-  </si>
-  <si>
-    <t>Improved Follower: You gain a level 3 follower. They are not restricted on their modifications. You can take this ability multiple times, each time gaining another level 3 follower. Alternatively, you could choose to advance a level 2 follower you already have to level 3 and then gain a new level 2 follower. Enabler.</t>
-  </si>
-  <si>
-    <t>Summon Sferic (8+ Intellect points): A sferic (Destiny, page 275) appears within a few days after you construct a simple beacon designed as a lure. If you apply an additional level of Effort as part of the call, the sferic is amenable to your instructions toward building an object or structure; otherwise, it acts according to its nature (which means it might still build something for you, but you risk havingyour mind plucked from your head when you make your request). The sferic remains until it finishes creating the structure you asked of it or it is attacked (in which case it defends itself and then leaves). Action to initiate, three days to construct beacon and summon sferic.</t>
-  </si>
-  <si>
-    <t>Scramble Machine (2 Intellect points): You render one machine within short range unable to function for one round. Alternatively, you can hinder any action by the machine (or by someone attempting to use the machine) for one minute. Action.</t>
-  </si>
-  <si>
-    <t>Interaction Skills: You are trained in two skills in which you are not already trained. Choose two of the following: deceiving, persuading, public speaking, seeing through deception, or intimidating. You can select this ability multiple times. Each time you select it, you must choose two different skills. Enabler.</t>
-  </si>
-  <si>
-    <t>Modify Cyphers: You can take any two cyphers and quickly jury-rig a new cypher of the same level as the lowest-level cypher. You determine the function of the new cypher, but it must be that of a cypher you have used before (but not necessarily one for which you have plans). The new cypher is a temperamental cypher, like those created with your Always Tinkering ability. The original two cyphers are consumed in this process. This ability does not function if one or more of the original cyphers are temperamental. Action.</t>
-  </si>
-  <si>
-    <t>Knowing the Weak Points: You gain +3 damage when attempting to damage a device, automaton, or other machine. Enabler.</t>
-  </si>
-  <si>
-    <t>Modify Artifact Function (5 Intellect points): You can take an artifact and any two cyphers and quickly jury-rig a new artifact of the level of the lowest-level cypher. You determine the function of the new artifact, but it must be that of an artifact or cypher you have used before (but not necessarily one for which you have plans). The GM sets the depletion of the new artifact, if applicable (it will usually be a bit worse than the original artifact). The two cyphers and the original artifact are consumed in this process. The original cyphers cannot be temperamental cyphers. Action.</t>
-  </si>
-  <si>
-    <t>Usurp Cypher: Choose one cypher that you carry. The cypher must have an effect that is not instantaneous. You destroy the cypher and gain its power, which functions for you continuously. You can choose a cypher when you gain this ability, or you can wait and make the choice later. However, once you usurp a cypher’s power, you cannot later switch to a different cypher—the ability works only once. Action to initiate.</t>
-  </si>
-  <si>
-    <t>Trigger Iotum Ray (1 Intellect point or iotum): If you have at least 1 unit of iotum, you can trigger it to release a short-range ray of force that inflicts 3 points of damage. This does not destroy the iotum. Alternatively, you can choose to have this destroy the iotum, in which case there is no Intellect cost. Action.</t>
-  </si>
-  <si>
-    <t>Knowledge Skills: You are trained in two skills in which you are not already trained. Choose two areas of knowledge such as history, geography, archeology, and so on. You can select this ability multiple times. Each time you select it, you must choose two different skills. Enabler.</t>
-  </si>
-  <si>
-    <t>Quick Armoring (4 Intellect points + io): You can siphon the residual energy in io (the eponymous iotum) to integrate and reinforce a layer of tightly wrapped clothing or encompassing cloaks that you wear. This requires at least one io, although it is not consumed in the process. For the next hour, you gain +2 to Armor. Action to initiate, one minute to complete.</t>
-  </si>
-  <si>
-    <t>Machine Bond: From very long range, you can activate and control a device (including an installation, automaton, or vehicle) that you have bonded with. For example, you can detonate a cypher even when it is held by someone else, or cause an installation turret to fire where you direct. Bonding is a process that requires 28 hours of meditation in the presence of the machine. Action.</t>
-  </si>
-  <si>
-    <t>Modify Artifact Power (6 Intellect points): You permanently add +1 to the level of an artifact of up to level 5. The difficulty of this task is equal to the modified higher level of the artifact. If the task is failed, the artifact makes a depletion roll and is not advanced in level. Once modified, the artifact can’t be similarly boosted again. Action.</t>
-  </si>
-  <si>
-    <t>Trained in Armor: You can wear armor for long periods of time without tiring and can compensate for slowed reactions from wearing armor. You can wear any kind of armor. You reduce the Speed Effort cost for wearing armor by 1. If you choose this as one of your starting inspired techniques, you start the game with armor of your choice. Enabler.</t>
-  </si>
-  <si>
-    <t>Make Do With Available Iotum (3+ Intellect points): Given an hour or so, you can figure out a way to substitute one kind of iotum called for in a plan with another kind of iotum, as long as the iotum you use is at least 1 level higher than the iotum originally called for. Alternatively, you can make do with 1 unit less than the number of units called for by the plan (to a minimum of 1 unit). For each additional level of Effort you apply, you can reduce the number by an additional unit, to a minimum of 1 unit. You can never substitute more than one kind of iotum per individual crafting task, though you could simultaneously substitute an iotum and decrease the number of units required by applying additional Effort. Action to initiate, one hour to complete.</t>
-  </si>
-  <si>
-    <t>Skill with Attacks: Choose one type of attack in which you are not already trained: light bashing, light bladed, light ranged, medium bashing, medium bladed, medium ranged, heavy bashing, heavy bladed, or heavy ranged. You are trained in attacks using that type of weapon. You can select this ability multiple times. Each time you select it, you must choose a different type of attack. Enabler.</t>
-  </si>
-  <si>
-    <t>Quick Mind Boost: You can siphon the residual energy in a single iotum to enhance your Intellect Edge by +1 for one minute. The iotum is destroyed. This ability does not allow you to enhance your Edge by more than +1. Action.</t>
-  </si>
-  <si>
-    <t>Town Pride: While you’re in a community that currently benefits from your Community Builder or Improved Community Builder special ability, your Might Edge, Speed Edge, and Intellect Edge all increase by 1. When you make a recovery roll in this community, you recover twice as many points. You can gain the benefit of this inspired technique even if you’re not in the community, as long as you have visited within the last three days. Enabler.</t>
+Artefact: You start with numenera plan of the artefact up to 1d6 + 4 level. This plan requires only half of resources to build the artefact. Chosen artefact plan is subject to GM approval.
+Inspired Techniques: Choose one of the following inspired techniques (or an inspired technique from a lower tier) to add to your repertoire. In addition, you can replace one of your lower-tier inspired techniques with a different inspired technique from the same lower tier.</t>
+  </si>
+  <si>
+    <t>Artefact: You start with numenera plan of the artefact up to 1d6 + 4 level. This plan requires only half of resources to build the artefact. Chosen artefact plan is subject to GM approval.
+Recruit Deputy: You gain a level 4 follower. They are not restricted on their modifications. Enabler.
+Inspired Techniques: Choose one of the following inspired techniques (or an inspired technique from a lower tier) to add to your repertoire. In addition, you can replace one of your lower-tier inspired techniques with a different inspired technique from the same lower tier.</t>
+  </si>
+  <si>
+    <t>Pools Starting Values: Might - 7, Speed - 9, Intellect - 12
+Bonus Pools Values: You get 6 additional points to divide among your stat Pools however you wish.
+Effort: Your Effort is 1.
+Genius: You have an Intellect Edge of 1, a Might Edge of 0, and a Speed Edge of 0.
+Expert Cypher Use: You can bear three cyphers at a time.
+Weapons: You can use light weapons without penalty. You have an inability with medium weapons and heavy weapons; your attacks with medium and heavy weapons are hindered.
+Skills: You are trained in understanding numenera, inability in salvaging numenera, inability crafting numenera.
+Starting Equipment: You start with clothing, one weapon, a book about the numenera, three cyphers (chosen for you by the GM), one oddity (chosen for you by the GM), and 4 shins (coins). Before selecting your weapons, armor, and other gear, you might want to wait until after you’ve chosen your esoteries, descriptor, and focus.
+Community Scholar: While you are present within a community, and actively and personally working on behalf of that community, the community’s health and infrastructure are both increased by +1. Enabler.
+Esoteries: You can tap into the numenera to reshape the world around you. Similar in appearance to the way a fabled wizard might seem to cast spells, these expressions of your knowledge are called esoteries. People who are not Nanos sometimes call them spells or charms.
+Most esoteries must be activated, which requires that you have a free hand and spend 1 or more Intellect points. If no Intellect point cost is given for an esotery, it functions continuously without needing to be activated. Some esoteries specify a duration, but you can always end one of your own esoteries anytime you wish.
+Choose two of the esoteries described below. You can’t choose the same esotery more than once unless its description says otherwise.
+Nano Player Intrusions: you can spend 1 XP to use one of the following player intrusions, provided the situation is appropriate and the GM agrees.
+- Advantageous Malfunction: a numenera device that is being used against you malfunctions. It might harm the user or one of their allies for a round, or activate a dramatic and distracting side effect for a few rounds.
+- Convenient Glimmer: a glimmer provides you with a clear answer or suggests a course of action with regard to an urgent question, problem, or obstacle you’re facing.
+- Inexplicably Unbroken: an inactive, ruined, or presumed-destroyed device temporarily activates and performs a useful function relevant to the situation. This is enough to buy you some time for a better solution, alleviate a complication that was interfering with your abilities, or just get you one more use out of a depleted cypher or artifact.</t>
+  </si>
+  <si>
+    <t>Esoteries: Choose one of the following esoteries (or an esotery from a lower tier) to add to your repertoire. In addition, you can replace one of your first-tier esoteries with a different first-tier esotery.</t>
+  </si>
+  <si>
+    <t>Adept Cypher Use: You can bear four cyphers at a time.
+Improved Community Scholar: A community continues to modify its health and infrastructure by +1 rank. However, you do not need to be constantly present in and actively working on behalf of the community for it to gain this benefit; it gains it merely because of your past efforts on the community’s behalf. Enabler. 
+Esoteries: Choose one of the following esoteries (or an esotery from a lower tier) to add to your repertoire. In addition, you can replace one of your lower-tier esoteries with a different esotery from the same lower tier.</t>
+  </si>
+  <si>
+    <t>Esoteries: Choose one of the following esoteries (or an esotery from a lower tier) to add to your repertoire. In addition, you can replace one of your lower-tier esoteries with a different esotery from the same lower tier.</t>
+  </si>
+  <si>
+    <t>Master Cypher Use: You can bear five cyphers at a time.
+Esoteries: Choose one of the following esoteries (or an esotery from a lower tier) to add to your repertoire. In addition, you can replace one of your lower-tier esoteries with a different esotery from the same lower tier.</t>
+  </si>
+  <si>
+    <t>Recruit Deputy: You gain a level 4 follower. They are not restricted on their modifications. Enabler.
+Esoteries: Choose one of the following esoteries (or an esotery from a lower tier) to add to your repertoire. In addition, you can replace one of your lower-tier esoteries with a different esotery from the same lower tier.</t>
+  </si>
+  <si>
+    <t>Pools Starting Values: Might - 11, Speed - 10, Intellect - 7
+Bonus Pools Values: You get 6 additional points to divide among your stat Pools however you wish.
+Effort: Your Effort is 1.
+Fighter: You have a Might Edge of 1, a Speed Edge of 1, and an Intellect Edge of 0.
+Combat Prowess: You add +1 damage to one type of attack of your choice: melee attacks or ranged attacks. Enabler.
+Cypher Use: You can bear two cyphers at a time.
+Trained in Armor: You can wear armor for long periods of time without tiring and can compensate for slowed reactions from wearing armor. You reduce the Speed Effort cost for wearing armor by 1. Enabler.
+Weapons: You can use any weapon without penalty.
+Physical Skills: Choose one of the following skills in which you aren’t already trained: balancing, climbing, jumping, or swimming. You are trained in this skill. You have an inability in crafting numenera, salvaging numenera, and understanding numenera.
+Starting Equipment: You start with clothing, two weapons (or one weapon and a shield), light or medium armor, an explorer’s pack, two cyphers (chosen for you by the GM), one oddity (chosen for you by the GM), and 5 shins (coins). If you start with a ranged weapon that requires ammunition (arrows, for example), you start with 12 of that type of ammunition. Before selecting your weapons, armor, and other gear, you might want to wait until after you’ve chosen your fighting moves, descriptor, and focus.
+Community Defender: While you are present within a community, and actively and personally working on behalf of that community, the community’s effective rank for damage inflicted is +1. Enabler. 
+Fighting Moves: You have a special talent for combat and can perform feats that others can barely imagine. These feats are called fighting moves. Some fighting moves are constant, ongoing effects, and others are specific actions that usually cost points from one of your stat Pools.
+Choose two of the fighting moves described below. You can’t choose the same fighting move more than once unless its description says otherwise.
+Player Intrusions: you can spend 1XP to use one of the following player intrusions, provided the situation is appropriate and the GM agrees. 
+- Perfect Setup: you’re fighting at least three foes and each one is standing in exactly the right spot for you to use a move you trained in long ago, allowing you to attack all three as a single action. Make a separate attack roll for each foe. You remain limited by the amount of Effort you can apply on one action. 
+- Old Friend: a comrade in arms from your past shows up unexpectedly and provides aid in whatever you’re doing. They are on a mission of their own and can’t stay longer than it takes to help out, chat a while after, and perhaps share a quick meal. 
+- Weapon Break: your foe’s weapon has a weak spot and in the course of the combat quickly becomes damaged and moves two steps down the object damage track.</t>
+  </si>
+  <si>
+    <t>Skill With Attacks: Choose one type of attack in which you are not already trained: light bashing, light bladed, light ranged, medium bashing, medium bladed, medium ranged, heavy bashing, heavy bladed, or heavy ranged. You are trained in attacks using that type of weapon. Enabler.
+Fighting Moves: Choose one of the following fighting moves (or a move from a lower tier) to add to your repertoire. In addition, you can replace one of your first-tier fighting moves with a different first-tier fighting move.</t>
+  </si>
+  <si>
+    <t>Expert Cypher Use: You can bear three cyphers at a time.
+Skill With Attacks: Choose one type of attack in which you are not already trained: light bashing, light bladed, light ranged, medium bashing, medium bladed, medium ranged, heavy bashing, heavy bladed, or heavy ranged. You are trained in attacks using that type of weapon. Enabler.
+Improved Community Defender: A community continues to modify its effective rank for damage inflicted by +1. However, you do not need to be constantly present in and actively working on behalf of the community for it to gain this benefit; it gains it merely because of your past defense of the community. Enabler. 
+Fighting Moves: Choose one of the following fighting moves (or a move from a lower tier) to add to your repertoire. In addition, you can also replace one of your lower-tier fighting moves with a different fighting move from the same lower tier.</t>
+  </si>
+  <si>
+    <t>Skill With Attacks: Choose one type of attack in which you are not already trained: light bashing, light bladed, light ranged, medium bashing, medium bladed, medium ranged, heavy bashing, heavy bladed, or heavy ranged. You are trained in attacks using that type of weapon. Enabler.
+Fighting Moves: Choose one of the following fighting moves (or a move from a lower tier) to add to your repertoire. In addition, you can also replace one of your lower-tier fighting moves with a different fighting move from the same lower tier.</t>
+  </si>
+  <si>
+    <t>Adept Cypher Use: You can bear four cyphers at a time.
+Mastery With Attacks: Choose one type of attack in which you are trained: light bashing, light bladed, light ranged, medium bashing, medium bladed, medium ranged, heavy bashing, heavy bladed, or heavy ranged. You are specialized in attacks using that type of weapon. Enabler. (In place of this ability, you may instead select Skill With Attacks to become trained in one type of attack.)
+Fighting Moves: Choose one of the following fighting moves (or a move from a lower tier) to add to your repertoire. In addition, you can also replace one of your lower-tier fighting moves with a different fighting move from the same lower tier.</t>
+  </si>
+  <si>
+    <t>Mastery With Attacks: Choose one type of attack in which you are trained: light bashing, light bladed, light ranged, medium bashing, medium bladed, medium ranged, heavy bashing, heavy bladed, or heavy ranged. You are specialized in attacks using that type of weapon. Enabler. (In place of this ability, you may instead select Skill With Attacks to become trained in one type of attack.)
+Choose one of the following:
+- Rampaging Beast Horde (12 Might points): You can take community actions with a horde or a community as if you were a rank 3 rampaging beast horde for one hour. You can spend a few rounds or minutes here and there taking character actions if something requires attention and still retain your horde status. For each allied PC that joins you and remains with you during this period who also spends 12 points from one of their Pools, you can extend the duration by one hour. Each point of damage you take while being treated as a rampaging beast horde is deducted from your Might Pool, or if you have allied PCs helping, the damage is split up and deducted from all your Might Pools evenly. Action to initiate. 
+- Recruit Deputy: You gain a level 4 follower. They are not restricted on their modifications. Enabler.
+Fighting Moves: Choose one of the following fighting moves (or a move from a lower tier) to add to your repertoire. In addition, you can also replace one of your lower-tier fighting moves with a different fighting move from the same lower tier.</t>
+  </si>
+  <si>
+    <t>Pools Starting Values: Might - 10, Speed - 10, Intellect - 10
+Bonus Pools Values: You get 6 additional points to divide among your stat Pools however you wish.
+Effort: Your Effort is 1.
+Jack of All Trades: You have an Edge of 1 for one stat of your choice: Might, Speed, or Intellect. You have an Edge of 0 for the other two stats.
+Cypher Use: You can bear two cyphers at a time.
+Weapons: You can use light and medium weapons without penalty. You have an inability with heavy weapons; your attacks with heavy weapons are hindered.
+Skills: Choose one skill (other than attacks or defense) in which you aren’t already trained. You are trained in this skill.
+Flex Skill: At the beginning of each day, choose one task (other than attacks or defense) on which you will concentrate. For the rest of that day, you’re trained in that task. You can’t use this ability with a skill you’re already trained in to become specialized.
+Starting Equipment: You start with clothing, two weapons, light armor, an explorer’s pack, a pack of light tools, two cyphers (chosen for you by the GM), one oddity (chosen by the GM), and 8 shins. Before selecting your weapons, armor, and other gear, you might want to wait until after you’ve chosen your tricks of the trade, descriptor, and focus.
+Community Fixer: While you are present within a community, and actively and personally working on behalf of that community, the community’s effective rank for health or infrastructure is increased by +1. You choose which is modified during any given community action. Enabler.Community Fixer: While you are present within a community, and actively and personally working on behalf of that community, the community’s effective rank for health or infrastructure is increased by +1. You choose which is modified during any given community action. Enabler.Community Fixer: While you are present within a community, and actively and personally working on behalf of that community, the community’s effective rank for health or infrastructure is increased by +1. You choose which is modified during any given community action. Enabler.
+Tricks of the Trade: You have a wide range of abilities that keep people guessing. Some of these tricks of the trade are technically esoteries, using the numenera, while others are more mundane. Some tricks are constant, ongoing effects; others are specific actions that usually cost points from one of your stat Pools.
+Choose two of the tricks described below. You can’t choose the same trick more than once unless its description says otherwise.
+Jack Player Intrusions: you can spend 1 XP to use one of the following player intrusions, provided the situation is appropriate and the GM agrees.
+- Familiar Insight: you know this person (or heard about them somewhere) well enough to give insight about their motives or intentions and how best to convince them to see things your way. You know the right words, posturing, inflection, amount of emotional manipulation, or even what sort of joke or agreeable complaint might sway them. This can convince a neutral person to take your side, or a hostile one to hear you out for a little while longer.
+- Inspirational Recall: you recall an important detail from a previous encounter (perhaps something you don’t even remember noticing at the time) that suggests a successful course of action for your current situation. This might be recognizing a password hidden in an innocuous code or riddle, realizing you saw a suspicious individual near a crime scene, overhearing an important conversation between two NPCs, or understanding that an NPC’s subtle glance or gesture had additional connotations indicating what you should do.
+- Lucky Break: something unexpected happens that is to your advantage. A rope your opponent is hanging from might snap, the person you’re debating in front of an influential Aeon Priest might trip or forget what they were going to say, or something that was supposed to last only a round or two lasts a little while longer.</t>
+  </si>
+  <si>
+    <t>Skills: You are trained in one task of your choosing (other than attacks or defense). If you choose a task you’re already trained in, you become specialized in that task. You can’t choose a task you’re already specialized in.
+Tricks of the Trade: Choose one of the following tricks (or a trick from a lower tier) to add to your repertoire. Instead of selecting a trick, you can select a lower-tier Glaive fighting move or Nano esotery. In addition, you can replace one of your first-tier tricks with a different first-tier trick.</t>
+  </si>
+  <si>
+    <t>Expert Cypher Use: You can bear three cyphers at a time.
+Skills: You are trained in one task of your choosing (other than attacks or defense). If you choose a task you’re already trained in, you become specialized in that task. You can’t choose a task you’re already specialized in.
+Improved Community Fixer: A community continues to modify its health or infrastructure by +1 rank. However, you do not need to be constantly present in and actively working on behalf of the community for it to gain this benefit; it gains it merely because of your past efforts on the community’s behalf. Whichever stat you modified last remains active until you return and modify it to something else. Enabler.
+Tricks of the Trade: Choose one of the following tricks (or a trick from a lower tier) to add to your repertoire. Instead of selecting a trick, you can select a lower-tier Glaive fighting move or Nano esotery. In addition, you can replace one of your lower-tier tricks with a different trick from the same lower tier.</t>
+  </si>
+  <si>
+    <t>Skills: You are trained in one task of your choosing (other than attacks or defense). If you choose a task you’re already trained in, you become specialized in that task. You can’t choose a task you’re already specialized in.
+Tricks of the Trade: Choose one of the following tricks (or a trick from a lower tier) to add to your repertoire. Instead of selecting a trick, you can select a lower-tier Glaive fighting move or Nano esotery. In addition, you can replace one of your lower-tier tricks with a different trick from the same lower tier.</t>
+  </si>
+  <si>
+    <t>Adept Cypher Use: You can bear four cyphers at a time.
+Skills: You are trained in one task of your choosing (other than attacks or defense). If you choose a task you’re already trained in, you become specialized in that task. You can’t choose a task you’re already specialized in.
+Tricks of the Trade: Choose one of the following tricks (or a trick from a lower tier) to add to your repertoire. Instead of selecting a trick, you can select a lower-tier Glaive fighting move or Nano esotery. In addition, you can replace one of your lower-tier tricks with a different trick from the same lower tier.</t>
+  </si>
+  <si>
+    <t>Skills: You are trained in one task of your choosing (other than attacks or defense). If you choose a task you’re already trained in, you become specialized in that task. You can’t choose a task you’re already specialized in.
+Recruit Deputy: You gain a level 4 follower. They are not restricted on their modifications. Enabler.
+Tricks of the Trade: Choose one of the following tricks (or a trick from a lower tier) to add to your repertoire. Instead of selecting a trick, you can select a lower-tier Glaive fighting move or Nano esotery. In addition, you can replace one of your lower-tier tricks with a different trick from the same lower tier.</t>
+  </si>
+  <si>
+    <t>Pools Starting Values: Might - 8, Speed - 9, Intellect - 11
+Bonus Pools Values: You get 6 additional points to divide among your stat Pools however you wish.
+Effort: Your Effort is 1.
+Leader: You have an Intellect Edge of 1, a Might Edge of 0, and a Speed Edge of 0.
+Cypher Use: You can bear two cyphers at a time.
+Weapons: You can use light weapons without penalty. You have an inability with medium and heavy weapons; your attacks with medium and heavy weapons are hindered.
+Interaction Skills: You are trained in two skills in which you are not already trained. Choose two of the following: persuasion, negotiation, deceiving, public speaking, seeing through deception, or intimidating. You have an inability in crafting numenera, salvaging numenera, and understanding numenera. Enabler.
+Community Leader: While you are present within a community, and actively and personally working on behalf of that community, the community’s rank is +1 for all purposes except damage inflicted. Enabler.
+Starting Equipment: You start with stylish clothing and a light weapon of your choice, two cyphers (chosen by the GM), one oddity, and 9 shins. If you start with a ranged weapon that requires ammunition (arrows, for example), you start with 12 of that type of ammunition. Before choosing your weapon and other gear, you might want to wait until after you’ve chosen your precepts, descriptor, and focus.
+Precepts: You have a wide range of abilities that give you an edge over other people. Some of these precepts are similar to esoteries in that you call upon a strange ability, use a device, and so on. Others are more mundane, relying on skill. Almost all require that you can speak to use them. Unless otherwise described, if they affect another creature, that creature must be able to perceive and understand you. Some precepts are constant, ongoing effects; others are specific actions that usually cost points from one of your stat Pools.
+Choose two of the precepts described below. You can’t choose the same precept more than once unless its description says otherwise. You can keep track of these in the Special Abilities section of your character sheet.
+Arkus Player Intrusions: you can spend 1 XP to use one of the following player intrusions,
+provided the situation is appropriate and the GM agrees.
+- Friendly NPC: an NPC you don’t know, someone you don’t know that well, or someone you know but who hasn’t been particularly friendly in the past chooses to help you, though doesn’t necessarily explain why. Maybe they’ll ask you for a favor in return afterward, depending on how much trouble they go to.
+- Perfect Suggestion: a follower or other already-friendly NPC suggests a course of action with regard to an urgent question, problem, or obstacle you’re facing.
+- Unexpected Gift: an NPC hands you a physical gift you were not expecting, one that helps put the situation at ease if things seem strained, or provides you with a new insight for understanding the context of the situation if there’s something you’re failing to understand or grasp.</t>
+  </si>
+  <si>
+    <t>Precepts: Choose one of the following Arkus precepts (or a precept from a lower tier) to add to your repertoire. In addition, you can replace one of your first-tier precepts with a different first-tier precept.</t>
+  </si>
+  <si>
+    <t>Expert Cypher Use: You can bear three cyphers at a time.
+Improved Community Leader: A community continues to modify its effective rank by +1 for any task except for attack and defense. However, you do not need to be constantly present in and actively working on behalf of the community for it to gain this benefit; it gains it merely because of your past work in the community. Enabler.
+Precepts: Choose one of the following Arkus precepts (or a precept from a lower tier) to add to your repertoire. In addition, you can replace one of your lower-tier precepts with a different precept from the same lower tier.</t>
+  </si>
+  <si>
+    <t>Precepts: Choose one of the following Arkus precepts (or a precept from a lower tier) to add to your repertoire. In addition, you can replace one of your lower-tier precepts with a different precept from the same lower tier.</t>
+  </si>
+  <si>
+    <t>Adept Cypher Use: You can bear four cyphers at a time.
+Precepts: Choose one of the following Arkus precepts (or a precept from a lower tier) to add to your repertoire. In addition, you can replace one of your lower-tier precepts with a different precept from the same lower tier.</t>
+  </si>
+  <si>
+    <t>Recruit Deputy: You gain a level 4 follower. They are not restricted on their modifications. Enabler. Alternatively, you can choose to advance a level 3 follower you already have to level 4 and then gain a new level 3 follower. Enabler.
+Precepts: Choose one of the following Arkus precepts (or a precept from a lower tier) to add to your repertoire. In addition, you can replace one of your lower-tier precepts with a different precept from the same lower tier.</t>
+  </si>
+  <si>
+    <t>Pools Starting Values: Might - 9, Speed - 9, Intellect - 10
+Bonus Pools Values: You get 6 additional points to divide among your stat Pools however you wish.
+Effort: Your Effort is 1.
+Talented: You have an Intellect Edge of 1, a Speed Edge of 1, and a Might Edge of 0.
+Cypher Use: You can bear two cyphers at a time.
+Weapons: You can use light and medium weapons without penalty. You have an inability with heavy weapons; your attacks with heavy weapons are hindered.
+Skills: You are trained in salvaging numenera. In addition, you are trained in an exploration skill in which you are not already trained. Choose from the following: navigation, perception, sensing danger, creature knowledge, initiative, peacefully opening communications with strangers, or tracking. You have an inability in crafting numenera and understanding numenera. Enabler.
+Community Explorer: While you are present within a community, and actively and personally working on behalf of that community, the community’s effective rank for purposes of finding resources, locating new trade routes, knowing about conditions just beyond the community, and detecting sneak attacks by enemies is +1. Enabler.
+Starting Equipment: You start with clothing,  two weapons (or one weapon and a shield), light armor or 1 extra unit of responsive synth (your choice), a pack of light tools, an explorer’s pack, two cyphers (chosen by the GM), one oddity (chosen by the GM), and 3 shins (coins). If you start with a ranged weapon that requires ammunition (arrows, for example), you start with 12 of that type of ammunition. Before selecting your weapons, armor, and other gear, you might want to wait until after you’ve chosen your Delve lore, descriptor, and focus.
+Delve Lore: You have special abilities called Delve lore that are related to exploring strange places and using numenera. Some of these abilities are constant, ongoing effects, and others are specific actions that usually cost points from one of your stat Pools.
+Choose two of the lores described below. You can’t choose the same lore more than once unless its description says otherwise. You can keep track of these in the Special Abilities section of your character sheet.
+Delve Player Intrusions: you can spend 1 XP to use one of the following player intrusions, provided the situation is appropriate and the GM agrees.
+- Fortuitous Malfunction: a trap or a dangerous device malfunctions before it can affect you.
+- Serendipitous Landmark: just when it seems like the path is lost, or you are, a trail marker, landmark, or simply the way the terrain or corridor bends, rises, or falls away suggests to you the best path forward, at least from this point.
+- Weak Strain: the poison or disease turns out not to be as debilitating or deadly as it first seemed, and inflicts only half the damage that it would have otherwise.</t>
+  </si>
+  <si>
+    <t>Delve Lore: Choose one of the following lores (or a lore from a lower tier) to add to your repertoire. In addition, you can replace one of your first-tier lores with a different first-tier lore.</t>
+  </si>
+  <si>
+    <t>Expert Cypher Use: You can bear three cyphers at a time.
+Improved Community Explorer: A community continues to modify its rank by +1 on any task that involves finding resources, locating new trade routes, knowing about conditions just beyond the community, and detecting sneak attacks by enemies. However, you do not need to be constantly present in and actively working on behalf of the community for it to gain this benefit; it gains it merely because of your past efforts in the community. Enabler.
+Delve Lore: Choose one of the following lores (or a lore from a lower tier) to add to your repertoire. In addition, you can replace one of your lower-tier lores with a different lower-tier lore.</t>
+  </si>
+  <si>
+    <t>Adept Cypher Use: You can bear four cyphers at a time.
+Refine Iotum: When you discover iotum on an initial salvage task, your follow-up attempts to locate a specific variety of iotum gain one free level of Effort if you use at least one level of Effort (maximum six levels). Enabler.
+Delve Lore: Choose one of the following lores (or a lore from a lower tier) to add to your repertoire. In addition, you can replace one of your lower-tier lores with a different lower-tier lore.</t>
+  </si>
+  <si>
+    <t>Recruit Deputy: You gain a level 4 follower. They are not restricted on their modifications. Enabler.
+Delve Lore: Choose one of the following lores (or a lore from a lower tier) to add to your repertoire. In addition, you can replace one of your lower-tier lores with a different lower-tier lore.</t>
+  </si>
+  <si>
+    <t>Iotum Cache: Whenever you find or salvage iotum, you gain additional salvage attempt to get iotum of specific kind. Enabler.
+Delve Lore: Choose one of the following lores (or a lore from a lower tier) to add to your repertoire. In addition, you can replace one of your lower-tier lores with a different lower-tier lore.</t>
+  </si>
+  <si>
+    <t>Deconstruct (3 Intellect points): You take the time to closely study a bit of scrap, machine, cypher, artifact, or other numenera object or structure before attempting to salvage iotum from it. If the salvage source possesses iotum that can be salvaged (as determined by the GM) you gain additional salvage attempt to get iotum of specific kind. Action to initiate, ten minutes to complete.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1467,7 +1463,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1524,7 +1520,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1945,12 +1940,12 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="97.5703125" style="1" customWidth="1"/>
@@ -1961,7 +1956,7 @@
     <col min="8" max="16384" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1984,295 +1979,299 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="409.6">
+    <row r="2" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="6"/>
+      <c r="B2" s="21" t="s">
+        <v>352</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>353</v>
+      </c>
       <c r="D2" s="9" t="s">
+        <v>354</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>355</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>356</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="189" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="10"/>
-      <c r="F2" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="D3" s="8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="189">
-      <c r="A3" s="7" t="s">
+      <c r="E3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="F3" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="G3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="8" t="s">
+    </row>
+    <row r="4" spans="1:7" ht="173.25" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="C4" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="D4" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="E4" s="8" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="173.25">
-      <c r="A4" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="8" t="s">
+      <c r="F4" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="G4" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="8" t="s">
+    </row>
+    <row r="5" spans="1:7" ht="126" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="C5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="D5" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="E5" s="8" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="126">
-      <c r="A5" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="8" t="s">
+      <c r="F5" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="G5" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="11" t="s">
+    </row>
+    <row r="6" spans="1:7" ht="189" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="C6" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="D6" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="E6" s="8" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="189">
-      <c r="A6" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="8" t="s">
+      <c r="F6" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="G6" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="8" t="s">
+    </row>
+    <row r="7" spans="1:7" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="C7" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="D7" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="E7" s="8" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="110.25">
-      <c r="A7" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="8" t="s">
+      <c r="F7" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="G7" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="8" t="s">
+    </row>
+    <row r="8" spans="1:7" ht="141.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="C8" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="D8" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="E8" s="10" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="141.75">
-      <c r="A8" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="10" t="s">
+      <c r="F8" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="G8" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="12" t="s">
+    </row>
+    <row r="9" spans="1:7" ht="157.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="C9" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="D9" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="E9" s="10" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="157.5">
-      <c r="A9" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="10" t="s">
+      <c r="F9" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="G9" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="D9" s="10" t="s">
+    </row>
+    <row r="10" spans="1:7" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="C10" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="D10" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="E10" s="10" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="78.75">
-      <c r="A10" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="10" t="s">
+      <c r="F10" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="G10" s="10"/>
+    </row>
+    <row r="11" spans="1:7" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="C11" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="D11" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="E11" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="G10" s="10"/>
-    </row>
-    <row r="11" spans="1:7" ht="110.25">
-      <c r="A11" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="10" t="s">
+      <c r="F11" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="G11" s="10"/>
+    </row>
+    <row r="12" spans="1:7" ht="126" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="C12" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="D12" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="E12" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="G11" s="10"/>
-    </row>
-    <row r="12" spans="1:7" ht="126">
-      <c r="A12" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="10" t="s">
+      <c r="F12" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="G12" s="10"/>
+    </row>
+    <row r="13" spans="1:7" ht="173.25" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="C13" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="D13" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="E13" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="G12" s="10"/>
-    </row>
-    <row r="13" spans="1:7" ht="173.25">
-      <c r="A13" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="10" t="s">
+      <c r="F13" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="G13" s="10"/>
+    </row>
+    <row r="14" spans="1:7" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="C14" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="D14" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="E14" s="10" t="s">
         <v>74</v>
-      </c>
-      <c r="G13" s="10"/>
-    </row>
-    <row r="14" spans="1:7" ht="110.25">
-      <c r="A14" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>78</v>
       </c>
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
     </row>
-    <row r="15" spans="1:7" s="2" customFormat="1" ht="47.25">
+    <row r="15" spans="1:7" s="2" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C15" s="13"/>
       <c r="D15" s="10"/>
@@ -2296,13 +2295,13 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="topRight" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomRight" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="115.5703125" style="1" customWidth="1"/>
@@ -2314,7 +2313,7 @@
     <col min="8" max="16384" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2337,308 +2336,308 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="409.6">
+    <row r="2" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="22" t="s">
+        <v>358</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>359</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>361</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>362</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="63" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="E3" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="F3" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="G3" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="F2" s="10" t="s">
+    </row>
+    <row r="4" spans="1:7" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="C4" s="8" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="63">
-      <c r="A3" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="8" t="s">
+      <c r="D4" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="E4" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="F4" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="G4" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="F3" s="9" t="s">
+    </row>
+    <row r="5" spans="1:7" ht="204.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="C5" s="8" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="110.25">
-      <c r="A4" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="11" t="s">
+      <c r="D5" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="E5" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="F5" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="G5" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="F4" s="8" t="s">
+    </row>
+    <row r="6" spans="1:7" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="C6" s="8" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="204.75">
-      <c r="A5" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="8" t="s">
+      <c r="D6" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="E6" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="F6" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="G6" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="F5" s="8" t="s">
+    </row>
+    <row r="7" spans="1:7" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="C7" s="14" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="94.5">
-      <c r="A6" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="8" t="s">
+      <c r="D7" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="E7" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="F7" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="G7" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="F6" s="8" t="s">
+    </row>
+    <row r="8" spans="1:7" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="C8" s="14" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="78.75">
-      <c r="A7" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="14" t="s">
+      <c r="D8" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="E8" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="F8" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="G8" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="F7" s="8" t="s">
+    </row>
+    <row r="9" spans="1:7" ht="63" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="C9" s="10" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="78.75">
-      <c r="A8" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="8" t="s">
+      <c r="D9" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="E9" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="F9" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="G9" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="F8" s="10" t="s">
+    </row>
+    <row r="10" spans="1:7" ht="63" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="C10" s="10" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="63">
-      <c r="A9" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="10" t="s">
+      <c r="D10" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="E10" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="F10" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="G10" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="F9" s="10" t="s">
+    </row>
+    <row r="11" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="C11" s="10" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="63">
-      <c r="A10" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="12" t="s">
+      <c r="D11" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="E11" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="F11" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="G11" s="10"/>
+    </row>
+    <row r="12" spans="1:7" ht="63" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="C12" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="D12" s="10" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="47.25">
-      <c r="A11" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="10" t="s">
+      <c r="E12" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="F12" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="G12" s="10"/>
+    </row>
+    <row r="13" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="C13" s="10" t="s">
         <v>136</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="G11" s="10"/>
-    </row>
-    <row r="12" spans="1:7" ht="63">
-      <c r="A12" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>140</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="G12" s="10"/>
-    </row>
-    <row r="13" spans="1:7" ht="47.25">
-      <c r="A13" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>143</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>144</v>
       </c>
       <c r="D13" s="10"/>
       <c r="E13" s="8" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
     </row>
-    <row r="14" spans="1:7" ht="78.75">
+    <row r="14" spans="1:7" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
     </row>
-    <row r="15" spans="1:7" ht="31.5">
+    <row r="15" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
       <c r="F15" s="10"/>
       <c r="G15" s="10"/>
     </row>
-    <row r="16" spans="1:7" ht="47.25">
+    <row r="16" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
@@ -2646,12 +2645,12 @@
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
     </row>
-    <row r="17" spans="1:7" s="2" customFormat="1" ht="31.5">
+    <row r="17" spans="1:7" s="2" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="C17" s="10"/>
       <c r="D17" s="13"/>
@@ -2673,12 +2672,12 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="topRight" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="97.5703125" style="1" customWidth="1"/>
@@ -2689,7 +2688,7 @@
     <col min="8" max="16384" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2712,335 +2711,335 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="409.6">
+    <row r="2" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="21" t="s">
+        <v>364</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>365</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>366</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>367</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>368</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="141.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="220.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="E4" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="F4" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="F2" s="10" t="s">
+      <c r="G4" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="G2" s="10" t="s">
+    </row>
+    <row r="5" spans="1:7" ht="126" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="8" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="141.75">
-      <c r="A3" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="8" t="s">
+      <c r="C5" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="D5" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="E5" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="F5" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="G5" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="F3" s="9" t="s">
+    </row>
+    <row r="6" spans="1:7" ht="141.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="C6" s="8" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="220.5">
-      <c r="A4" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="8" t="s">
+      <c r="D6" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="E6" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="F6" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="G6" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="F4" s="8" t="s">
+    </row>
+    <row r="7" spans="1:7" ht="141.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="D7" s="10" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="126">
-      <c r="A5" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="8" t="s">
+      <c r="E7" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="F7" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="D5" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="E5" s="8" t="s">
+      <c r="G7" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="F5" s="8" t="s">
+    </row>
+    <row r="8" spans="1:7" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="C8" s="8" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="141.75">
-      <c r="A6" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="8" t="s">
+      <c r="D8" s="10" t="s">
         <v>174</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="E8" s="10" t="s">
         <v>175</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="F8" s="10" t="s">
         <v>176</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="G8" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="F6" s="8" t="s">
+    </row>
+    <row r="9" spans="1:7" ht="63" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="8" t="s">
         <v>178</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="C9" s="8" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="141.75">
-      <c r="A7" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="C7" s="8" t="s">
+      <c r="D9" s="10" t="s">
         <v>180</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="E9" s="12" t="s">
         <v>181</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="F9" s="10" t="s">
         <v>182</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="G9" s="10" t="s">
         <v>183</v>
       </c>
-      <c r="G7" s="8" t="s">
+    </row>
+    <row r="10" spans="1:7" ht="157.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="8" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="94.5">
-      <c r="A8" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="8" t="s">
+      <c r="C10" s="10" t="s">
         <v>185</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="D10" s="10" t="s">
         <v>186</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="E10" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="F10" s="10" t="s">
         <v>188</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="G10" s="10" t="s">
         <v>189</v>
       </c>
-      <c r="G8" s="8" t="s">
+    </row>
+    <row r="11" spans="1:7" ht="157.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="10" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="63">
-      <c r="A9" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="8" t="s">
+      <c r="C11" s="12" t="s">
         <v>191</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="D11" s="10" t="s">
         <v>192</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="E11" s="10" t="s">
         <v>193</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="F11" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="G11" s="10" t="s">
         <v>195</v>
       </c>
-      <c r="G9" s="10" t="s">
+    </row>
+    <row r="12" spans="1:7" ht="63" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="C12" s="10" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="157.5">
-      <c r="A10" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="8" t="s">
+      <c r="D12" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="E12" s="10" t="s">
         <v>197</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>198</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>199</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>200</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>201</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="157.5">
-      <c r="A11" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>203</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>204</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>205</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>206</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="G11" s="10" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="63">
-      <c r="A12" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>143</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>209</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>210</v>
       </c>
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
     </row>
-    <row r="13" spans="1:7" ht="31.5">
+    <row r="13" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>211</v>
+        <v>198</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
     </row>
-    <row r="14" spans="1:7" ht="47.25">
+    <row r="14" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>214</v>
+        <v>201</v>
       </c>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
     </row>
-    <row r="15" spans="1:7" ht="63">
+    <row r="15" spans="1:7" ht="63" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>215</v>
+        <v>202</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
       <c r="F15" s="10"/>
       <c r="G15" s="10"/>
     </row>
-    <row r="16" spans="1:7" s="2" customFormat="1" ht="63">
+    <row r="16" spans="1:7" s="2" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>217</v>
+        <v>204</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
     </row>
-    <row r="17" spans="1:7" ht="47.25">
+    <row r="17" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B17" s="13"/>
       <c r="C17" s="12" t="s">
-        <v>218</v>
+        <v>205</v>
       </c>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
     </row>
-    <row r="18" spans="1:7" ht="63">
+    <row r="18" spans="1:7" ht="63" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B18" s="13"/>
       <c r="C18" s="10" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
       <c r="D18" s="13"/>
       <c r="E18" s="10"/>
@@ -3062,11 +3061,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.7109375" style="3" customWidth="1"/>
     <col min="2" max="2" width="91" style="3" customWidth="1"/>
@@ -3078,7 +3077,7 @@
     <col min="8" max="16384" width="11.5703125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -3101,243 +3100,247 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="409.6">
+    <row r="2" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="23" t="s">
+        <v>370</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>371</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>372</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>373</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>374</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>207</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>209</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>210</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>213</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>216</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>218</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>219</v>
+      </c>
+      <c r="D5" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12" t="s">
+      <c r="E5" s="12" t="s">
         <v>221</v>
       </c>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12" t="s">
+      <c r="F5" s="12" t="s">
         <v>222</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G5" s="12" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="92.25" customHeight="1">
-      <c r="A3" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="12" t="s">
+    <row r="6" spans="1:7" ht="63" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="12" t="s">
         <v>224</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C6" s="12" t="s">
         <v>225</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D6" s="12" t="s">
         <v>226</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E6" s="12" t="s">
         <v>227</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F6" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="G6" s="12" t="s">
         <v>228</v>
       </c>
-      <c r="G3" s="12" t="s">
+    </row>
+    <row r="7" spans="1:7" ht="141.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="12" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="110.25">
-      <c r="A4" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>115</v>
-      </c>
-      <c r="C4" s="12" t="s">
+      <c r="C7" s="12" t="s">
         <v>230</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D7" s="12" t="s">
         <v>231</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E7" s="12" t="s">
         <v>232</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F7" s="12" t="s">
         <v>233</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G7" s="12" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="110.25">
-      <c r="A5" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="12" t="s">
+    <row r="8" spans="1:7" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="12" t="s">
         <v>235</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C8" s="12" t="s">
         <v>236</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D8" s="12" t="s">
         <v>237</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E8" s="12" t="s">
         <v>238</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F8" s="12" t="s">
         <v>239</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G8" s="12" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="63">
-      <c r="A6" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="12" t="s">
+    <row r="9" spans="1:7" ht="126" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="12" t="s">
         <v>241</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C9" s="12" t="s">
         <v>242</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D9" s="12" t="s">
         <v>243</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E9" s="12" t="s">
         <v>244</v>
       </c>
-      <c r="F6" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="G6" s="12" t="s">
+      <c r="G9" s="12" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="141.75">
-      <c r="A7" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="12" t="s">
+    <row r="10" spans="1:7" ht="126" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="12" t="s">
         <v>246</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C10" s="12" t="s">
         <v>247</v>
       </c>
-      <c r="D7" s="12" t="s">
-        <v>248</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>249</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>250</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="110.25">
-      <c r="A8" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>252</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>253</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>254</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>255</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>256</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="126">
-      <c r="A9" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>258</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>259</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>260</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>261</v>
-      </c>
-      <c r="G9" s="12" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="126">
-      <c r="A10" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>263</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>264</v>
-      </c>
       <c r="D10" s="12" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="F10" s="12"/>
       <c r="G10" s="12" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="157.5">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>266</v>
+        <v>249</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>268</v>
+        <v>251</v>
       </c>
       <c r="E11" s="12"/>
       <c r="F11" s="12"/>
       <c r="G11" s="14" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="47.25">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>270</v>
+        <v>253</v>
       </c>
       <c r="C12" s="12"/>
       <c r="D12" s="12" t="s">
-        <v>271</v>
+        <v>254</v>
       </c>
       <c r="E12" s="12"/>
       <c r="F12" s="12"/>
     </row>
-    <row r="13" spans="1:7" ht="94.5">
+    <row r="13" spans="1:7" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>272</v>
+        <v>255</v>
       </c>
       <c r="C13" s="12"/>
       <c r="D13" s="12"/>
@@ -3345,12 +3348,12 @@
       <c r="F13" s="12"/>
       <c r="G13" s="12"/>
     </row>
-    <row r="14" spans="1:7" ht="63">
+    <row r="14" spans="1:7" ht="63" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>273</v>
+        <v>256</v>
       </c>
       <c r="C14" s="12"/>
       <c r="D14" s="12"/>
@@ -3358,12 +3361,12 @@
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
     </row>
-    <row r="15" spans="1:7" ht="78.75">
+    <row r="15" spans="1:7" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>274</v>
+        <v>257</v>
       </c>
       <c r="C15" s="12"/>
       <c r="D15" s="12"/>
@@ -3371,12 +3374,12 @@
       <c r="F15" s="12"/>
       <c r="G15" s="12"/>
     </row>
-    <row r="16" spans="1:7" ht="94.5">
+    <row r="16" spans="1:7" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>275</v>
+        <v>258</v>
       </c>
       <c r="C16" s="12"/>
       <c r="D16" s="12"/>
@@ -3400,14 +3403,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.7109375" style="3" customWidth="1"/>
     <col min="2" max="2" width="106.7109375" style="3" customWidth="1"/>
@@ -3419,7 +3422,7 @@
     <col min="8" max="16384" width="11.5703125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -3442,280 +3445,282 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="409.6">
+    <row r="2" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="23" t="s">
+        <v>376</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>377</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>378</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>381</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>379</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>259</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>260</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>261</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>262</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>263</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>267</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>268</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="362.25" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>270</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>273</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="63" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>275</v>
+      </c>
+      <c r="D6" s="12" t="s">
         <v>276</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12" t="s">
+      <c r="E6" s="12" t="s">
         <v>277</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="F6" s="12" t="s">
         <v>278</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="G6" s="12" t="s">
         <v>279</v>
       </c>
-      <c r="G2" s="12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="94.5">
-      <c r="A3" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="14" t="s">
+    </row>
+    <row r="7" spans="1:7" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="12" t="s">
         <v>280</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C7" s="12" t="s">
         <v>281</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D7" s="12" t="s">
         <v>282</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E7" s="12" t="s">
         <v>283</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F7" s="12" t="s">
         <v>284</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G7" s="12" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="110.25">
-      <c r="A4" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="12" t="s">
+    <row r="8" spans="1:7" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="12" t="s">
         <v>286</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C8" s="12" t="s">
+        <v>382</v>
+      </c>
+      <c r="D8" s="12" t="s">
         <v>287</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="E8" s="12" t="s">
         <v>288</v>
       </c>
-      <c r="E4" s="12" t="s">
-        <v>194</v>
-      </c>
-      <c r="F4" s="12" t="s">
+      <c r="F8" s="12" t="s">
         <v>289</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G8" s="12" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="362.25">
-      <c r="A5" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="12" t="s">
+    <row r="9" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="C9" s="12" t="s">
         <v>291</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="D9" s="18" t="s">
         <v>292</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>293</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>294</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>201</v>
-      </c>
-      <c r="G5" s="12" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="63">
-      <c r="A6" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>203</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>296</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>297</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>298</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>299</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="78.75">
-      <c r="A7" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>301</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>302</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>303</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>304</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>305</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="94.5">
-      <c r="A8" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>307</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>308</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>309</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>310</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>311</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="31.5">
-      <c r="A9" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>109</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>313</v>
-      </c>
-      <c r="D9" s="18" t="s">
-        <v>314</v>
       </c>
       <c r="E9" s="12"/>
       <c r="F9" s="12" t="s">
-        <v>315</v>
+        <v>293</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="63">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="63" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>317</v>
+        <v>295</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>318</v>
+        <v>296</v>
       </c>
       <c r="E10" s="12"/>
       <c r="F10" s="12" t="s">
-        <v>319</v>
+        <v>297</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="47.25">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>321</v>
+        <v>299</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E11" s="12"/>
       <c r="F11" s="12"/>
       <c r="G11" s="12"/>
     </row>
-    <row r="12" spans="1:7" ht="78.75">
+    <row r="12" spans="1:7" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>322</v>
+        <v>300</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>323</v>
+        <v>301</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>324</v>
+        <v>302</v>
       </c>
       <c r="E12" s="12"/>
       <c r="F12" s="12"/>
       <c r="G12" s="12"/>
     </row>
-    <row r="13" spans="1:7" ht="47.25">
+    <row r="13" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="D13" s="12"/>
       <c r="E13" s="12"/>
       <c r="F13" s="12"/>
       <c r="G13" s="12"/>
     </row>
-    <row r="14" spans="1:7" ht="126">
+    <row r="14" spans="1:7" ht="126" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>325</v>
+        <v>303</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>326</v>
+        <v>304</v>
       </c>
       <c r="D14" s="12"/>
       <c r="E14" s="12"/>
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
     </row>
-    <row r="15" spans="1:7" s="4" customFormat="1" ht="110.25">
+    <row r="15" spans="1:7" s="4" customFormat="1" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>327</v>
+        <v>305</v>
       </c>
       <c r="D15" s="12"/>
       <c r="E15" s="12"/>
@@ -3737,11 +3742,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.7109375" style="19" customWidth="1"/>
     <col min="2" max="2" width="106.7109375" style="19" customWidth="1"/>
@@ -3753,7 +3758,7 @@
     <col min="8" max="16384" width="11.5703125" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3776,194 +3781,194 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="409.6">
+    <row r="2" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="21" t="s">
+        <v>346</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>347</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>348</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>349</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>350</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>306</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>307</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>308</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>309</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>310</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>312</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>313</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>314</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>315</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>316</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="141.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>318</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>319</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>320</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>321</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>322</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>324</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>325</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>326</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>327</v>
+      </c>
+      <c r="F6" s="10" t="s">
         <v>328</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="G6" s="10" t="s">
         <v>329</v>
       </c>
-      <c r="D2" s="10" t="s">
+    </row>
+    <row r="7" spans="1:7" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="10" t="s">
         <v>330</v>
       </c>
-      <c r="E2" s="10" t="s">
-        <v>329</v>
-      </c>
-      <c r="F2" s="10" t="s">
+      <c r="C7" s="10" t="s">
         <v>331</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="D7" s="10" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="110.25">
-      <c r="A3" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="10" t="s">
+      <c r="E7" s="10" t="s">
         <v>333</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="F7" s="10" t="s">
         <v>334</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="G7" s="10" t="s">
         <v>335</v>
       </c>
-      <c r="E3" s="10" t="s">
+    </row>
+    <row r="8" spans="1:7" s="20" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="10" t="s">
         <v>336</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="C8" s="10" t="s">
         <v>337</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="D8" s="10" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="94.5">
-      <c r="A4" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="10" t="s">
+      <c r="E8" s="10" t="s">
         <v>339</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="F8" s="10" t="s">
         <v>340</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="G8" s="10"/>
+    </row>
+    <row r="9" spans="1:7" ht="126" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="24" t="s">
         <v>341</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="C9" s="10" t="s">
         <v>342</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="D9" s="10" t="s">
         <v>343</v>
-      </c>
-      <c r="G4" s="10" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="141.75">
-      <c r="A5" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>345</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>346</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>347</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>348</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>349</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="110.25">
-      <c r="A6" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>351</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>352</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>353</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>354</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>355</v>
-      </c>
-      <c r="G6" s="10" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="94.5">
-      <c r="A7" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>357</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>358</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>359</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>360</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>361</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" s="21" customFormat="1" ht="63">
-      <c r="A8" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>363</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>364</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>365</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>366</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>367</v>
-      </c>
-      <c r="G8" s="10"/>
-    </row>
-    <row r="9" spans="1:7" ht="126">
-      <c r="A9" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="25" t="s">
-        <v>368</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>369</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>370</v>
       </c>
       <c r="E9" s="10"/>
       <c r="F9" s="10" t="s">
-        <v>371</v>
+        <v>344</v>
       </c>
       <c r="G9" s="10"/>
     </row>
-    <row r="10" spans="1:7" ht="78.75">
+    <row r="10" spans="1:7" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B10" s="13"/>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
       <c r="F10" s="10" t="s">
-        <v>372</v>
+        <v>345</v>
       </c>
       <c r="G10" s="10"/>
     </row>

</xml_diff>